<commit_message>
Add m102.4-like Fv seq
</commit_message>
<xml_diff>
--- a/candidates.xlsx
+++ b/candidates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Documents\GitHub\Nipah_gpG_Fv_Generation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6156EF-19A9-4001-AD43-2E8D5DB5B68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0706BEC8-B4DD-489F-AF75-702328E45FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>antigen_id</t>
   </si>
@@ -166,13 +166,28 @@
   </si>
   <si>
     <t>DIQLTQSPFLSLSPGSTASISCSGSSYDYTSGYRYKSSGKSPKPWMQRFLYSGSKRFSGVPERFIGSGTDFALTISRVEAEDVGFCSGWIFPFTFGPGTKVDIK</t>
+  </si>
+  <si>
+    <t>General LLM</t>
+  </si>
+  <si>
+    <t>Qwen3-235B-A22B-Instruct-2507</t>
+  </si>
+  <si>
+    <t>sbio-nipahgpg-008</t>
+  </si>
+  <si>
+    <t>QVQLVESGGGVVQPGRSLRLSCAASGFTFSSYAMSWVRQAPGKGLEWVSAIWSNGGSTYYADSVKGRFTISRDNAKNSLYLQMNSLRAEDTAVYYCARDYGSYGYFDYWGQGTLVTVSS</t>
+  </si>
+  <si>
+    <t>DIVMTQSPLSLPVTPGEPASISCRSSQSLLYSNGNTYLEWYLQKPGQSPQLLIYLVSKLDSGVPDRFSGSGSGTDFTLKISRVEAEDLGIYYCQQSKEVPYTFGAGTKLEIK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -191,6 +206,13 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -213,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -227,11 +249,63 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -619,17 +693,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMJ11"/>
+  <dimension ref="A1:AMJ10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="54" style="2" customWidth="1"/>
     <col min="6" max="6" width="42.140625" style="2" customWidth="1"/>
@@ -639,36 +713,1051 @@
     <col min="10" max="1024" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="5"/>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+      <c r="AU1" s="5"/>
+      <c r="AV1" s="5"/>
+      <c r="AW1" s="5"/>
+      <c r="AX1" s="5"/>
+      <c r="AY1" s="5"/>
+      <c r="AZ1" s="5"/>
+      <c r="BA1" s="5"/>
+      <c r="BB1" s="5"/>
+      <c r="BC1" s="5"/>
+      <c r="BD1" s="5"/>
+      <c r="BE1" s="5"/>
+      <c r="BF1" s="5"/>
+      <c r="BG1" s="5"/>
+      <c r="BH1" s="5"/>
+      <c r="BI1" s="5"/>
+      <c r="BJ1" s="5"/>
+      <c r="BK1" s="5"/>
+      <c r="BL1" s="5"/>
+      <c r="BM1" s="5"/>
+      <c r="BN1" s="5"/>
+      <c r="BO1" s="5"/>
+      <c r="BP1" s="5"/>
+      <c r="BQ1" s="5"/>
+      <c r="BR1" s="5"/>
+      <c r="BS1" s="5"/>
+      <c r="BT1" s="5"/>
+      <c r="BU1" s="5"/>
+      <c r="BV1" s="5"/>
+      <c r="BW1" s="5"/>
+      <c r="BX1" s="5"/>
+      <c r="BY1" s="5"/>
+      <c r="BZ1" s="5"/>
+      <c r="CA1" s="5"/>
+      <c r="CB1" s="5"/>
+      <c r="CC1" s="5"/>
+      <c r="CD1" s="5"/>
+      <c r="CE1" s="5"/>
+      <c r="CF1" s="5"/>
+      <c r="CG1" s="5"/>
+      <c r="CH1" s="5"/>
+      <c r="CI1" s="5"/>
+      <c r="CJ1" s="5"/>
+      <c r="CK1" s="5"/>
+      <c r="CL1" s="5"/>
+      <c r="CM1" s="5"/>
+      <c r="CN1" s="5"/>
+      <c r="CO1" s="5"/>
+      <c r="CP1" s="5"/>
+      <c r="CQ1" s="5"/>
+      <c r="CR1" s="5"/>
+      <c r="CS1" s="5"/>
+      <c r="CT1" s="5"/>
+      <c r="CU1" s="5"/>
+      <c r="CV1" s="5"/>
+      <c r="CW1" s="5"/>
+      <c r="CX1" s="5"/>
+      <c r="CY1" s="5"/>
+      <c r="CZ1" s="5"/>
+      <c r="DA1" s="5"/>
+      <c r="DB1" s="5"/>
+      <c r="DC1" s="5"/>
+      <c r="DD1" s="5"/>
+      <c r="DE1" s="5"/>
+      <c r="DF1" s="5"/>
+      <c r="DG1" s="5"/>
+      <c r="DH1" s="5"/>
+      <c r="DI1" s="5"/>
+      <c r="DJ1" s="5"/>
+      <c r="DK1" s="5"/>
+      <c r="DL1" s="5"/>
+      <c r="DM1" s="5"/>
+      <c r="DN1" s="5"/>
+      <c r="DO1" s="5"/>
+      <c r="DP1" s="5"/>
+      <c r="DQ1" s="5"/>
+      <c r="DR1" s="5"/>
+      <c r="DS1" s="5"/>
+      <c r="DT1" s="5"/>
+      <c r="DU1" s="5"/>
+      <c r="DV1" s="5"/>
+      <c r="DW1" s="5"/>
+      <c r="DX1" s="5"/>
+      <c r="DY1" s="5"/>
+      <c r="DZ1" s="5"/>
+      <c r="EA1" s="5"/>
+      <c r="EB1" s="5"/>
+      <c r="EC1" s="5"/>
+      <c r="ED1" s="5"/>
+      <c r="EE1" s="5"/>
+      <c r="EF1" s="5"/>
+      <c r="EG1" s="5"/>
+      <c r="EH1" s="5"/>
+      <c r="EI1" s="5"/>
+      <c r="EJ1" s="5"/>
+      <c r="EK1" s="5"/>
+      <c r="EL1" s="5"/>
+      <c r="EM1" s="5"/>
+      <c r="EN1" s="5"/>
+      <c r="EO1" s="5"/>
+      <c r="EP1" s="5"/>
+      <c r="EQ1" s="5"/>
+      <c r="ER1" s="5"/>
+      <c r="ES1" s="5"/>
+      <c r="ET1" s="5"/>
+      <c r="EU1" s="5"/>
+      <c r="EV1" s="5"/>
+      <c r="EW1" s="5"/>
+      <c r="EX1" s="5"/>
+      <c r="EY1" s="5"/>
+      <c r="EZ1" s="5"/>
+      <c r="FA1" s="5"/>
+      <c r="FB1" s="5"/>
+      <c r="FC1" s="5"/>
+      <c r="FD1" s="5"/>
+      <c r="FE1" s="5"/>
+      <c r="FF1" s="5"/>
+      <c r="FG1" s="5"/>
+      <c r="FH1" s="5"/>
+      <c r="FI1" s="5"/>
+      <c r="FJ1" s="5"/>
+      <c r="FK1" s="5"/>
+      <c r="FL1" s="5"/>
+      <c r="FM1" s="5"/>
+      <c r="FN1" s="5"/>
+      <c r="FO1" s="5"/>
+      <c r="FP1" s="5"/>
+      <c r="FQ1" s="5"/>
+      <c r="FR1" s="5"/>
+      <c r="FS1" s="5"/>
+      <c r="FT1" s="5"/>
+      <c r="FU1" s="5"/>
+      <c r="FV1" s="5"/>
+      <c r="FW1" s="5"/>
+      <c r="FX1" s="5"/>
+      <c r="FY1" s="5"/>
+      <c r="FZ1" s="5"/>
+      <c r="GA1" s="5"/>
+      <c r="GB1" s="5"/>
+      <c r="GC1" s="5"/>
+      <c r="GD1" s="5"/>
+      <c r="GE1" s="5"/>
+      <c r="GF1" s="5"/>
+      <c r="GG1" s="5"/>
+      <c r="GH1" s="5"/>
+      <c r="GI1" s="5"/>
+      <c r="GJ1" s="5"/>
+      <c r="GK1" s="5"/>
+      <c r="GL1" s="5"/>
+      <c r="GM1" s="5"/>
+      <c r="GN1" s="5"/>
+      <c r="GO1" s="5"/>
+      <c r="GP1" s="5"/>
+      <c r="GQ1" s="5"/>
+      <c r="GR1" s="5"/>
+      <c r="GS1" s="5"/>
+      <c r="GT1" s="5"/>
+      <c r="GU1" s="5"/>
+      <c r="GV1" s="5"/>
+      <c r="GW1" s="5"/>
+      <c r="GX1" s="5"/>
+      <c r="GY1" s="5"/>
+      <c r="GZ1" s="5"/>
+      <c r="HA1" s="5"/>
+      <c r="HB1" s="5"/>
+      <c r="HC1" s="5"/>
+      <c r="HD1" s="5"/>
+      <c r="HE1" s="5"/>
+      <c r="HF1" s="5"/>
+      <c r="HG1" s="5"/>
+      <c r="HH1" s="5"/>
+      <c r="HI1" s="5"/>
+      <c r="HJ1" s="5"/>
+      <c r="HK1" s="5"/>
+      <c r="HL1" s="5"/>
+      <c r="HM1" s="5"/>
+      <c r="HN1" s="5"/>
+      <c r="HO1" s="5"/>
+      <c r="HP1" s="5"/>
+      <c r="HQ1" s="5"/>
+      <c r="HR1" s="5"/>
+      <c r="HS1" s="5"/>
+      <c r="HT1" s="5"/>
+      <c r="HU1" s="5"/>
+      <c r="HV1" s="5"/>
+      <c r="HW1" s="5"/>
+      <c r="HX1" s="5"/>
+      <c r="HY1" s="5"/>
+      <c r="HZ1" s="5"/>
+      <c r="IA1" s="5"/>
+      <c r="IB1" s="5"/>
+      <c r="IC1" s="5"/>
+      <c r="ID1" s="5"/>
+      <c r="IE1" s="5"/>
+      <c r="IF1" s="5"/>
+      <c r="IG1" s="5"/>
+      <c r="IH1" s="5"/>
+      <c r="II1" s="5"/>
+      <c r="IJ1" s="5"/>
+      <c r="IK1" s="5"/>
+      <c r="IL1" s="5"/>
+      <c r="IM1" s="5"/>
+      <c r="IN1" s="5"/>
+      <c r="IO1" s="5"/>
+      <c r="IP1" s="5"/>
+      <c r="IQ1" s="5"/>
+      <c r="IR1" s="5"/>
+      <c r="IS1" s="5"/>
+      <c r="IT1" s="5"/>
+      <c r="IU1" s="5"/>
+      <c r="IV1" s="5"/>
+      <c r="IW1" s="5"/>
+      <c r="IX1" s="5"/>
+      <c r="IY1" s="5"/>
+      <c r="IZ1" s="5"/>
+      <c r="JA1" s="5"/>
+      <c r="JB1" s="5"/>
+      <c r="JC1" s="5"/>
+      <c r="JD1" s="5"/>
+      <c r="JE1" s="5"/>
+      <c r="JF1" s="5"/>
+      <c r="JG1" s="5"/>
+      <c r="JH1" s="5"/>
+      <c r="JI1" s="5"/>
+      <c r="JJ1" s="5"/>
+      <c r="JK1" s="5"/>
+      <c r="JL1" s="5"/>
+      <c r="JM1" s="5"/>
+      <c r="JN1" s="5"/>
+      <c r="JO1" s="5"/>
+      <c r="JP1" s="5"/>
+      <c r="JQ1" s="5"/>
+      <c r="JR1" s="5"/>
+      <c r="JS1" s="5"/>
+      <c r="JT1" s="5"/>
+      <c r="JU1" s="5"/>
+      <c r="JV1" s="5"/>
+      <c r="JW1" s="5"/>
+      <c r="JX1" s="5"/>
+      <c r="JY1" s="5"/>
+      <c r="JZ1" s="5"/>
+      <c r="KA1" s="5"/>
+      <c r="KB1" s="5"/>
+      <c r="KC1" s="5"/>
+      <c r="KD1" s="5"/>
+      <c r="KE1" s="5"/>
+      <c r="KF1" s="5"/>
+      <c r="KG1" s="5"/>
+      <c r="KH1" s="5"/>
+      <c r="KI1" s="5"/>
+      <c r="KJ1" s="5"/>
+      <c r="KK1" s="5"/>
+      <c r="KL1" s="5"/>
+      <c r="KM1" s="5"/>
+      <c r="KN1" s="5"/>
+      <c r="KO1" s="5"/>
+      <c r="KP1" s="5"/>
+      <c r="KQ1" s="5"/>
+      <c r="KR1" s="5"/>
+      <c r="KS1" s="5"/>
+      <c r="KT1" s="5"/>
+      <c r="KU1" s="5"/>
+      <c r="KV1" s="5"/>
+      <c r="KW1" s="5"/>
+      <c r="KX1" s="5"/>
+      <c r="KY1" s="5"/>
+      <c r="KZ1" s="5"/>
+      <c r="LA1" s="5"/>
+      <c r="LB1" s="5"/>
+      <c r="LC1" s="5"/>
+      <c r="LD1" s="5"/>
+      <c r="LE1" s="5"/>
+      <c r="LF1" s="5"/>
+      <c r="LG1" s="5"/>
+      <c r="LH1" s="5"/>
+      <c r="LI1" s="5"/>
+      <c r="LJ1" s="5"/>
+      <c r="LK1" s="5"/>
+      <c r="LL1" s="5"/>
+      <c r="LM1" s="5"/>
+      <c r="LN1" s="5"/>
+      <c r="LO1" s="5"/>
+      <c r="LP1" s="5"/>
+      <c r="LQ1" s="5"/>
+      <c r="LR1" s="5"/>
+      <c r="LS1" s="5"/>
+      <c r="LT1" s="5"/>
+      <c r="LU1" s="5"/>
+      <c r="LV1" s="5"/>
+      <c r="LW1" s="5"/>
+      <c r="LX1" s="5"/>
+      <c r="LY1" s="5"/>
+      <c r="LZ1" s="5"/>
+      <c r="MA1" s="5"/>
+      <c r="MB1" s="5"/>
+      <c r="MC1" s="5"/>
+      <c r="MD1" s="5"/>
+      <c r="ME1" s="5"/>
+      <c r="MF1" s="5"/>
+      <c r="MG1" s="5"/>
+      <c r="MH1" s="5"/>
+      <c r="MI1" s="5"/>
+      <c r="MJ1" s="5"/>
+      <c r="MK1" s="5"/>
+      <c r="ML1" s="5"/>
+      <c r="MM1" s="5"/>
+      <c r="MN1" s="5"/>
+      <c r="MO1" s="5"/>
+      <c r="MP1" s="5"/>
+      <c r="MQ1" s="5"/>
+      <c r="MR1" s="5"/>
+      <c r="MS1" s="5"/>
+      <c r="MT1" s="5"/>
+      <c r="MU1" s="5"/>
+      <c r="MV1" s="5"/>
+      <c r="MW1" s="5"/>
+      <c r="MX1" s="5"/>
+      <c r="MY1" s="5"/>
+      <c r="MZ1" s="5"/>
+      <c r="NA1" s="5"/>
+      <c r="NB1" s="5"/>
+      <c r="NC1" s="5"/>
+      <c r="ND1" s="5"/>
+      <c r="NE1" s="5"/>
+      <c r="NF1" s="5"/>
+      <c r="NG1" s="5"/>
+      <c r="NH1" s="5"/>
+      <c r="NI1" s="5"/>
+      <c r="NJ1" s="5"/>
+      <c r="NK1" s="5"/>
+      <c r="NL1" s="5"/>
+      <c r="NM1" s="5"/>
+      <c r="NN1" s="5"/>
+      <c r="NO1" s="5"/>
+      <c r="NP1" s="5"/>
+      <c r="NQ1" s="5"/>
+      <c r="NR1" s="5"/>
+      <c r="NS1" s="5"/>
+      <c r="NT1" s="5"/>
+      <c r="NU1" s="5"/>
+      <c r="NV1" s="5"/>
+      <c r="NW1" s="5"/>
+      <c r="NX1" s="5"/>
+      <c r="NY1" s="5"/>
+      <c r="NZ1" s="5"/>
+      <c r="OA1" s="5"/>
+      <c r="OB1" s="5"/>
+      <c r="OC1" s="5"/>
+      <c r="OD1" s="5"/>
+      <c r="OE1" s="5"/>
+      <c r="OF1" s="5"/>
+      <c r="OG1" s="5"/>
+      <c r="OH1" s="5"/>
+      <c r="OI1" s="5"/>
+      <c r="OJ1" s="5"/>
+      <c r="OK1" s="5"/>
+      <c r="OL1" s="5"/>
+      <c r="OM1" s="5"/>
+      <c r="ON1" s="5"/>
+      <c r="OO1" s="5"/>
+      <c r="OP1" s="5"/>
+      <c r="OQ1" s="5"/>
+      <c r="OR1" s="5"/>
+      <c r="OS1" s="5"/>
+      <c r="OT1" s="5"/>
+      <c r="OU1" s="5"/>
+      <c r="OV1" s="5"/>
+      <c r="OW1" s="5"/>
+      <c r="OX1" s="5"/>
+      <c r="OY1" s="5"/>
+      <c r="OZ1" s="5"/>
+      <c r="PA1" s="5"/>
+      <c r="PB1" s="5"/>
+      <c r="PC1" s="5"/>
+      <c r="PD1" s="5"/>
+      <c r="PE1" s="5"/>
+      <c r="PF1" s="5"/>
+      <c r="PG1" s="5"/>
+      <c r="PH1" s="5"/>
+      <c r="PI1" s="5"/>
+      <c r="PJ1" s="5"/>
+      <c r="PK1" s="5"/>
+      <c r="PL1" s="5"/>
+      <c r="PM1" s="5"/>
+      <c r="PN1" s="5"/>
+      <c r="PO1" s="5"/>
+      <c r="PP1" s="5"/>
+      <c r="PQ1" s="5"/>
+      <c r="PR1" s="5"/>
+      <c r="PS1" s="5"/>
+      <c r="PT1" s="5"/>
+      <c r="PU1" s="5"/>
+      <c r="PV1" s="5"/>
+      <c r="PW1" s="5"/>
+      <c r="PX1" s="5"/>
+      <c r="PY1" s="5"/>
+      <c r="PZ1" s="5"/>
+      <c r="QA1" s="5"/>
+      <c r="QB1" s="5"/>
+      <c r="QC1" s="5"/>
+      <c r="QD1" s="5"/>
+      <c r="QE1" s="5"/>
+      <c r="QF1" s="5"/>
+      <c r="QG1" s="5"/>
+      <c r="QH1" s="5"/>
+      <c r="QI1" s="5"/>
+      <c r="QJ1" s="5"/>
+      <c r="QK1" s="5"/>
+      <c r="QL1" s="5"/>
+      <c r="QM1" s="5"/>
+      <c r="QN1" s="5"/>
+      <c r="QO1" s="5"/>
+      <c r="QP1" s="5"/>
+      <c r="QQ1" s="5"/>
+      <c r="QR1" s="5"/>
+      <c r="QS1" s="5"/>
+      <c r="QT1" s="5"/>
+      <c r="QU1" s="5"/>
+      <c r="QV1" s="5"/>
+      <c r="QW1" s="5"/>
+      <c r="QX1" s="5"/>
+      <c r="QY1" s="5"/>
+      <c r="QZ1" s="5"/>
+      <c r="RA1" s="5"/>
+      <c r="RB1" s="5"/>
+      <c r="RC1" s="5"/>
+      <c r="RD1" s="5"/>
+      <c r="RE1" s="5"/>
+      <c r="RF1" s="5"/>
+      <c r="RG1" s="5"/>
+      <c r="RH1" s="5"/>
+      <c r="RI1" s="5"/>
+      <c r="RJ1" s="5"/>
+      <c r="RK1" s="5"/>
+      <c r="RL1" s="5"/>
+      <c r="RM1" s="5"/>
+      <c r="RN1" s="5"/>
+      <c r="RO1" s="5"/>
+      <c r="RP1" s="5"/>
+      <c r="RQ1" s="5"/>
+      <c r="RR1" s="5"/>
+      <c r="RS1" s="5"/>
+      <c r="RT1" s="5"/>
+      <c r="RU1" s="5"/>
+      <c r="RV1" s="5"/>
+      <c r="RW1" s="5"/>
+      <c r="RX1" s="5"/>
+      <c r="RY1" s="5"/>
+      <c r="RZ1" s="5"/>
+      <c r="SA1" s="5"/>
+      <c r="SB1" s="5"/>
+      <c r="SC1" s="5"/>
+      <c r="SD1" s="5"/>
+      <c r="SE1" s="5"/>
+      <c r="SF1" s="5"/>
+      <c r="SG1" s="5"/>
+      <c r="SH1" s="5"/>
+      <c r="SI1" s="5"/>
+      <c r="SJ1" s="5"/>
+      <c r="SK1" s="5"/>
+      <c r="SL1" s="5"/>
+      <c r="SM1" s="5"/>
+      <c r="SN1" s="5"/>
+      <c r="SO1" s="5"/>
+      <c r="SP1" s="5"/>
+      <c r="SQ1" s="5"/>
+      <c r="SR1" s="5"/>
+      <c r="SS1" s="5"/>
+      <c r="ST1" s="5"/>
+      <c r="SU1" s="5"/>
+      <c r="SV1" s="5"/>
+      <c r="SW1" s="5"/>
+      <c r="SX1" s="5"/>
+      <c r="SY1" s="5"/>
+      <c r="SZ1" s="5"/>
+      <c r="TA1" s="5"/>
+      <c r="TB1" s="5"/>
+      <c r="TC1" s="5"/>
+      <c r="TD1" s="5"/>
+      <c r="TE1" s="5"/>
+      <c r="TF1" s="5"/>
+      <c r="TG1" s="5"/>
+      <c r="TH1" s="5"/>
+      <c r="TI1" s="5"/>
+      <c r="TJ1" s="5"/>
+      <c r="TK1" s="5"/>
+      <c r="TL1" s="5"/>
+      <c r="TM1" s="5"/>
+      <c r="TN1" s="5"/>
+      <c r="TO1" s="5"/>
+      <c r="TP1" s="5"/>
+      <c r="TQ1" s="5"/>
+      <c r="TR1" s="5"/>
+      <c r="TS1" s="5"/>
+      <c r="TT1" s="5"/>
+      <c r="TU1" s="5"/>
+      <c r="TV1" s="5"/>
+      <c r="TW1" s="5"/>
+      <c r="TX1" s="5"/>
+      <c r="TY1" s="5"/>
+      <c r="TZ1" s="5"/>
+      <c r="UA1" s="5"/>
+      <c r="UB1" s="5"/>
+      <c r="UC1" s="5"/>
+      <c r="UD1" s="5"/>
+      <c r="UE1" s="5"/>
+      <c r="UF1" s="5"/>
+      <c r="UG1" s="5"/>
+      <c r="UH1" s="5"/>
+      <c r="UI1" s="5"/>
+      <c r="UJ1" s="5"/>
+      <c r="UK1" s="5"/>
+      <c r="UL1" s="5"/>
+      <c r="UM1" s="5"/>
+      <c r="UN1" s="5"/>
+      <c r="UO1" s="5"/>
+      <c r="UP1" s="5"/>
+      <c r="UQ1" s="5"/>
+      <c r="UR1" s="5"/>
+      <c r="US1" s="5"/>
+      <c r="UT1" s="5"/>
+      <c r="UU1" s="5"/>
+      <c r="UV1" s="5"/>
+      <c r="UW1" s="5"/>
+      <c r="UX1" s="5"/>
+      <c r="UY1" s="5"/>
+      <c r="UZ1" s="5"/>
+      <c r="VA1" s="5"/>
+      <c r="VB1" s="5"/>
+      <c r="VC1" s="5"/>
+      <c r="VD1" s="5"/>
+      <c r="VE1" s="5"/>
+      <c r="VF1" s="5"/>
+      <c r="VG1" s="5"/>
+      <c r="VH1" s="5"/>
+      <c r="VI1" s="5"/>
+      <c r="VJ1" s="5"/>
+      <c r="VK1" s="5"/>
+      <c r="VL1" s="5"/>
+      <c r="VM1" s="5"/>
+      <c r="VN1" s="5"/>
+      <c r="VO1" s="5"/>
+      <c r="VP1" s="5"/>
+      <c r="VQ1" s="5"/>
+      <c r="VR1" s="5"/>
+      <c r="VS1" s="5"/>
+      <c r="VT1" s="5"/>
+      <c r="VU1" s="5"/>
+      <c r="VV1" s="5"/>
+      <c r="VW1" s="5"/>
+      <c r="VX1" s="5"/>
+      <c r="VY1" s="5"/>
+      <c r="VZ1" s="5"/>
+      <c r="WA1" s="5"/>
+      <c r="WB1" s="5"/>
+      <c r="WC1" s="5"/>
+      <c r="WD1" s="5"/>
+      <c r="WE1" s="5"/>
+      <c r="WF1" s="5"/>
+      <c r="WG1" s="5"/>
+      <c r="WH1" s="5"/>
+      <c r="WI1" s="5"/>
+      <c r="WJ1" s="5"/>
+      <c r="WK1" s="5"/>
+      <c r="WL1" s="5"/>
+      <c r="WM1" s="5"/>
+      <c r="WN1" s="5"/>
+      <c r="WO1" s="5"/>
+      <c r="WP1" s="5"/>
+      <c r="WQ1" s="5"/>
+      <c r="WR1" s="5"/>
+      <c r="WS1" s="5"/>
+      <c r="WT1" s="5"/>
+      <c r="WU1" s="5"/>
+      <c r="WV1" s="5"/>
+      <c r="WW1" s="5"/>
+      <c r="WX1" s="5"/>
+      <c r="WY1" s="5"/>
+      <c r="WZ1" s="5"/>
+      <c r="XA1" s="5"/>
+      <c r="XB1" s="5"/>
+      <c r="XC1" s="5"/>
+      <c r="XD1" s="5"/>
+      <c r="XE1" s="5"/>
+      <c r="XF1" s="5"/>
+      <c r="XG1" s="5"/>
+      <c r="XH1" s="5"/>
+      <c r="XI1" s="5"/>
+      <c r="XJ1" s="5"/>
+      <c r="XK1" s="5"/>
+      <c r="XL1" s="5"/>
+      <c r="XM1" s="5"/>
+      <c r="XN1" s="5"/>
+      <c r="XO1" s="5"/>
+      <c r="XP1" s="5"/>
+      <c r="XQ1" s="5"/>
+      <c r="XR1" s="5"/>
+      <c r="XS1" s="5"/>
+      <c r="XT1" s="5"/>
+      <c r="XU1" s="5"/>
+      <c r="XV1" s="5"/>
+      <c r="XW1" s="5"/>
+      <c r="XX1" s="5"/>
+      <c r="XY1" s="5"/>
+      <c r="XZ1" s="5"/>
+      <c r="YA1" s="5"/>
+      <c r="YB1" s="5"/>
+      <c r="YC1" s="5"/>
+      <c r="YD1" s="5"/>
+      <c r="YE1" s="5"/>
+      <c r="YF1" s="5"/>
+      <c r="YG1" s="5"/>
+      <c r="YH1" s="5"/>
+      <c r="YI1" s="5"/>
+      <c r="YJ1" s="5"/>
+      <c r="YK1" s="5"/>
+      <c r="YL1" s="5"/>
+      <c r="YM1" s="5"/>
+      <c r="YN1" s="5"/>
+      <c r="YO1" s="5"/>
+      <c r="YP1" s="5"/>
+      <c r="YQ1" s="5"/>
+      <c r="YR1" s="5"/>
+      <c r="YS1" s="5"/>
+      <c r="YT1" s="5"/>
+      <c r="YU1" s="5"/>
+      <c r="YV1" s="5"/>
+      <c r="YW1" s="5"/>
+      <c r="YX1" s="5"/>
+      <c r="YY1" s="5"/>
+      <c r="YZ1" s="5"/>
+      <c r="ZA1" s="5"/>
+      <c r="ZB1" s="5"/>
+      <c r="ZC1" s="5"/>
+      <c r="ZD1" s="5"/>
+      <c r="ZE1" s="5"/>
+      <c r="ZF1" s="5"/>
+      <c r="ZG1" s="5"/>
+      <c r="ZH1" s="5"/>
+      <c r="ZI1" s="5"/>
+      <c r="ZJ1" s="5"/>
+      <c r="ZK1" s="5"/>
+      <c r="ZL1" s="5"/>
+      <c r="ZM1" s="5"/>
+      <c r="ZN1" s="5"/>
+      <c r="ZO1" s="5"/>
+      <c r="ZP1" s="5"/>
+      <c r="ZQ1" s="5"/>
+      <c r="ZR1" s="5"/>
+      <c r="ZS1" s="5"/>
+      <c r="ZT1" s="5"/>
+      <c r="ZU1" s="5"/>
+      <c r="ZV1" s="5"/>
+      <c r="ZW1" s="5"/>
+      <c r="ZX1" s="5"/>
+      <c r="ZY1" s="5"/>
+      <c r="ZZ1" s="5"/>
+      <c r="AAA1" s="5"/>
+      <c r="AAB1" s="5"/>
+      <c r="AAC1" s="5"/>
+      <c r="AAD1" s="5"/>
+      <c r="AAE1" s="5"/>
+      <c r="AAF1" s="5"/>
+      <c r="AAG1" s="5"/>
+      <c r="AAH1" s="5"/>
+      <c r="AAI1" s="5"/>
+      <c r="AAJ1" s="5"/>
+      <c r="AAK1" s="5"/>
+      <c r="AAL1" s="5"/>
+      <c r="AAM1" s="5"/>
+      <c r="AAN1" s="5"/>
+      <c r="AAO1" s="5"/>
+      <c r="AAP1" s="5"/>
+      <c r="AAQ1" s="5"/>
+      <c r="AAR1" s="5"/>
+      <c r="AAS1" s="5"/>
+      <c r="AAT1" s="5"/>
+      <c r="AAU1" s="5"/>
+      <c r="AAV1" s="5"/>
+      <c r="AAW1" s="5"/>
+      <c r="AAX1" s="5"/>
+      <c r="AAY1" s="5"/>
+      <c r="AAZ1" s="5"/>
+      <c r="ABA1" s="5"/>
+      <c r="ABB1" s="5"/>
+      <c r="ABC1" s="5"/>
+      <c r="ABD1" s="5"/>
+      <c r="ABE1" s="5"/>
+      <c r="ABF1" s="5"/>
+      <c r="ABG1" s="5"/>
+      <c r="ABH1" s="5"/>
+      <c r="ABI1" s="5"/>
+      <c r="ABJ1" s="5"/>
+      <c r="ABK1" s="5"/>
+      <c r="ABL1" s="5"/>
+      <c r="ABM1" s="5"/>
+      <c r="ABN1" s="5"/>
+      <c r="ABO1" s="5"/>
+      <c r="ABP1" s="5"/>
+      <c r="ABQ1" s="5"/>
+      <c r="ABR1" s="5"/>
+      <c r="ABS1" s="5"/>
+      <c r="ABT1" s="5"/>
+      <c r="ABU1" s="5"/>
+      <c r="ABV1" s="5"/>
+      <c r="ABW1" s="5"/>
+      <c r="ABX1" s="5"/>
+      <c r="ABY1" s="5"/>
+      <c r="ABZ1" s="5"/>
+      <c r="ACA1" s="5"/>
+      <c r="ACB1" s="5"/>
+      <c r="ACC1" s="5"/>
+      <c r="ACD1" s="5"/>
+      <c r="ACE1" s="5"/>
+      <c r="ACF1" s="5"/>
+      <c r="ACG1" s="5"/>
+      <c r="ACH1" s="5"/>
+      <c r="ACI1" s="5"/>
+      <c r="ACJ1" s="5"/>
+      <c r="ACK1" s="5"/>
+      <c r="ACL1" s="5"/>
+      <c r="ACM1" s="5"/>
+      <c r="ACN1" s="5"/>
+      <c r="ACO1" s="5"/>
+      <c r="ACP1" s="5"/>
+      <c r="ACQ1" s="5"/>
+      <c r="ACR1" s="5"/>
+      <c r="ACS1" s="5"/>
+      <c r="ACT1" s="5"/>
+      <c r="ACU1" s="5"/>
+      <c r="ACV1" s="5"/>
+      <c r="ACW1" s="5"/>
+      <c r="ACX1" s="5"/>
+      <c r="ACY1" s="5"/>
+      <c r="ACZ1" s="5"/>
+      <c r="ADA1" s="5"/>
+      <c r="ADB1" s="5"/>
+      <c r="ADC1" s="5"/>
+      <c r="ADD1" s="5"/>
+      <c r="ADE1" s="5"/>
+      <c r="ADF1" s="5"/>
+      <c r="ADG1" s="5"/>
+      <c r="ADH1" s="5"/>
+      <c r="ADI1" s="5"/>
+      <c r="ADJ1" s="5"/>
+      <c r="ADK1" s="5"/>
+      <c r="ADL1" s="5"/>
+      <c r="ADM1" s="5"/>
+      <c r="ADN1" s="5"/>
+      <c r="ADO1" s="5"/>
+      <c r="ADP1" s="5"/>
+      <c r="ADQ1" s="5"/>
+      <c r="ADR1" s="5"/>
+      <c r="ADS1" s="5"/>
+      <c r="ADT1" s="5"/>
+      <c r="ADU1" s="5"/>
+      <c r="ADV1" s="5"/>
+      <c r="ADW1" s="5"/>
+      <c r="ADX1" s="5"/>
+      <c r="ADY1" s="5"/>
+      <c r="ADZ1" s="5"/>
+      <c r="AEA1" s="5"/>
+      <c r="AEB1" s="5"/>
+      <c r="AEC1" s="5"/>
+      <c r="AED1" s="5"/>
+      <c r="AEE1" s="5"/>
+      <c r="AEF1" s="5"/>
+      <c r="AEG1" s="5"/>
+      <c r="AEH1" s="5"/>
+      <c r="AEI1" s="5"/>
+      <c r="AEJ1" s="5"/>
+      <c r="AEK1" s="5"/>
+      <c r="AEL1" s="5"/>
+      <c r="AEM1" s="5"/>
+      <c r="AEN1" s="5"/>
+      <c r="AEO1" s="5"/>
+      <c r="AEP1" s="5"/>
+      <c r="AEQ1" s="5"/>
+      <c r="AER1" s="5"/>
+      <c r="AES1" s="5"/>
+      <c r="AET1" s="5"/>
+      <c r="AEU1" s="5"/>
+      <c r="AEV1" s="5"/>
+      <c r="AEW1" s="5"/>
+      <c r="AEX1" s="5"/>
+      <c r="AEY1" s="5"/>
+      <c r="AEZ1" s="5"/>
+      <c r="AFA1" s="5"/>
+      <c r="AFB1" s="5"/>
+      <c r="AFC1" s="5"/>
+      <c r="AFD1" s="5"/>
+      <c r="AFE1" s="5"/>
+      <c r="AFF1" s="5"/>
+      <c r="AFG1" s="5"/>
+      <c r="AFH1" s="5"/>
+      <c r="AFI1" s="5"/>
+      <c r="AFJ1" s="5"/>
+      <c r="AFK1" s="5"/>
+      <c r="AFL1" s="5"/>
+      <c r="AFM1" s="5"/>
+      <c r="AFN1" s="5"/>
+      <c r="AFO1" s="5"/>
+      <c r="AFP1" s="5"/>
+      <c r="AFQ1" s="5"/>
+      <c r="AFR1" s="5"/>
+      <c r="AFS1" s="5"/>
+      <c r="AFT1" s="5"/>
+      <c r="AFU1" s="5"/>
+      <c r="AFV1" s="5"/>
+      <c r="AFW1" s="5"/>
+      <c r="AFX1" s="5"/>
+      <c r="AFY1" s="5"/>
+      <c r="AFZ1" s="5"/>
+      <c r="AGA1" s="5"/>
+      <c r="AGB1" s="5"/>
+      <c r="AGC1" s="5"/>
+      <c r="AGD1" s="5"/>
+      <c r="AGE1" s="5"/>
+      <c r="AGF1" s="5"/>
+      <c r="AGG1" s="5"/>
+      <c r="AGH1" s="5"/>
+      <c r="AGI1" s="5"/>
+      <c r="AGJ1" s="5"/>
+      <c r="AGK1" s="5"/>
+      <c r="AGL1" s="5"/>
+      <c r="AGM1" s="5"/>
+      <c r="AGN1" s="5"/>
+      <c r="AGO1" s="5"/>
+      <c r="AGP1" s="5"/>
+      <c r="AGQ1" s="5"/>
+      <c r="AGR1" s="5"/>
+      <c r="AGS1" s="5"/>
+      <c r="AGT1" s="5"/>
+      <c r="AGU1" s="5"/>
+      <c r="AGV1" s="5"/>
+      <c r="AGW1" s="5"/>
+      <c r="AGX1" s="5"/>
+      <c r="AGY1" s="5"/>
+      <c r="AGZ1" s="5"/>
+      <c r="AHA1" s="5"/>
+      <c r="AHB1" s="5"/>
+      <c r="AHC1" s="5"/>
+      <c r="AHD1" s="5"/>
+      <c r="AHE1" s="5"/>
+      <c r="AHF1" s="5"/>
+      <c r="AHG1" s="5"/>
+      <c r="AHH1" s="5"/>
+      <c r="AHI1" s="5"/>
+      <c r="AHJ1" s="5"/>
+      <c r="AHK1" s="5"/>
+      <c r="AHL1" s="5"/>
+      <c r="AHM1" s="5"/>
+      <c r="AHN1" s="5"/>
+      <c r="AHO1" s="5"/>
+      <c r="AHP1" s="5"/>
+      <c r="AHQ1" s="5"/>
+      <c r="AHR1" s="5"/>
+      <c r="AHS1" s="5"/>
+      <c r="AHT1" s="5"/>
+      <c r="AHU1" s="5"/>
+      <c r="AHV1" s="5"/>
+      <c r="AHW1" s="5"/>
+      <c r="AHX1" s="5"/>
+      <c r="AHY1" s="5"/>
+      <c r="AHZ1" s="5"/>
+      <c r="AIA1" s="5"/>
+      <c r="AIB1" s="5"/>
+      <c r="AIC1" s="5"/>
+      <c r="AID1" s="5"/>
+      <c r="AIE1" s="5"/>
+      <c r="AIF1" s="5"/>
+      <c r="AIG1" s="5"/>
+      <c r="AIH1" s="5"/>
+      <c r="AII1" s="5"/>
+      <c r="AIJ1" s="5"/>
+      <c r="AIK1" s="5"/>
+      <c r="AIL1" s="5"/>
+      <c r="AIM1" s="5"/>
+      <c r="AIN1" s="5"/>
+      <c r="AIO1" s="5"/>
+      <c r="AIP1" s="5"/>
+      <c r="AIQ1" s="5"/>
+      <c r="AIR1" s="5"/>
+      <c r="AIS1" s="5"/>
+      <c r="AIT1" s="5"/>
+      <c r="AIU1" s="5"/>
+      <c r="AIV1" s="5"/>
+      <c r="AIW1" s="5"/>
+      <c r="AIX1" s="5"/>
+      <c r="AIY1" s="5"/>
+      <c r="AIZ1" s="5"/>
+      <c r="AJA1" s="5"/>
+      <c r="AJB1" s="5"/>
+      <c r="AJC1" s="5"/>
+      <c r="AJD1" s="5"/>
+      <c r="AJE1" s="5"/>
+      <c r="AJF1" s="5"/>
+      <c r="AJG1" s="5"/>
+      <c r="AJH1" s="5"/>
+      <c r="AJI1" s="5"/>
+      <c r="AJJ1" s="5"/>
+      <c r="AJK1" s="5"/>
+      <c r="AJL1" s="5"/>
+      <c r="AJM1" s="5"/>
+      <c r="AJN1" s="5"/>
+      <c r="AJO1" s="5"/>
+      <c r="AJP1" s="5"/>
+      <c r="AJQ1" s="5"/>
+      <c r="AJR1" s="5"/>
+      <c r="AJS1" s="5"/>
+      <c r="AJT1" s="5"/>
+      <c r="AJU1" s="5"/>
+      <c r="AJV1" s="5"/>
+      <c r="AJW1" s="5"/>
+      <c r="AJX1" s="5"/>
+      <c r="AJY1" s="5"/>
+      <c r="AJZ1" s="5"/>
+      <c r="AKA1" s="5"/>
+      <c r="AKB1" s="5"/>
+      <c r="AKC1" s="5"/>
+      <c r="AKD1" s="5"/>
+      <c r="AKE1" s="5"/>
+      <c r="AKF1" s="5"/>
+      <c r="AKG1" s="5"/>
+      <c r="AKH1" s="5"/>
+      <c r="AKI1" s="5"/>
+      <c r="AKJ1" s="5"/>
+      <c r="AKK1" s="5"/>
+      <c r="AKL1" s="5"/>
+      <c r="AKM1" s="5"/>
+      <c r="AKN1" s="5"/>
+      <c r="AKO1" s="5"/>
+      <c r="AKP1" s="5"/>
+      <c r="AKQ1" s="5"/>
+      <c r="AKR1" s="5"/>
+      <c r="AKS1" s="5"/>
+      <c r="AKT1" s="5"/>
+      <c r="AKU1" s="5"/>
+      <c r="AKV1" s="5"/>
+      <c r="AKW1" s="5"/>
+      <c r="AKX1" s="5"/>
+      <c r="AKY1" s="5"/>
+      <c r="AKZ1" s="5"/>
+      <c r="ALA1" s="5"/>
+      <c r="ALB1" s="5"/>
+      <c r="ALC1" s="5"/>
+      <c r="ALD1" s="5"/>
+      <c r="ALE1" s="5"/>
+      <c r="ALF1" s="5"/>
+      <c r="ALG1" s="5"/>
+      <c r="ALH1" s="5"/>
+      <c r="ALI1" s="5"/>
+      <c r="ALJ1" s="5"/>
+      <c r="ALK1" s="5"/>
+      <c r="ALL1" s="5"/>
+      <c r="ALM1" s="5"/>
+      <c r="ALN1" s="5"/>
+      <c r="ALO1" s="5"/>
+      <c r="ALP1" s="5"/>
+      <c r="ALQ1" s="5"/>
+      <c r="ALR1" s="5"/>
+      <c r="ALS1" s="5"/>
+      <c r="ALT1" s="5"/>
+      <c r="ALU1" s="5"/>
+      <c r="ALV1" s="5"/>
+      <c r="ALW1" s="5"/>
+      <c r="ALX1" s="5"/>
+      <c r="ALY1" s="5"/>
+      <c r="ALZ1" s="5"/>
+      <c r="AMA1" s="5"/>
+      <c r="AMB1" s="5"/>
+      <c r="AMC1" s="5"/>
+      <c r="AMD1" s="5"/>
+      <c r="AME1" s="5"/>
+      <c r="AMF1" s="5"/>
+      <c r="AMG1" s="5"/>
+      <c r="AMH1" s="5"/>
+      <c r="AMI1" s="5"/>
+      <c r="AMJ1" s="5"/>
     </row>
-    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1024" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -700,7 +1789,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1024" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -732,7 +1821,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1024" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -764,7 +1853,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1024" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -796,7 +1885,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1024" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -828,7 +1917,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1024" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -848,15 +1937,15 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="str">
-        <f t="shared" ref="H7:H8" si="0">_xlfn.CONCAT(E7,"GGGSGGGSGGGSGGGS",F7)</f>
+        <f t="shared" ref="H7:H9" si="0">_xlfn.CONCAT(E7,"GGGSGGGSGGGSGGGS",F7)</f>
         <v>VGPRTTLTVSLRSGASVKMSCKASGYSFTWVRQKPGQGLEWVKISYDGLKDYTNYKFQGVKATITADKSSNTAYLQISNLTSEDTAVYFCSRRAVYYDYWGQGTTLTVSSGGGSGGGSGGGSGGGSVTVALGTVSLAPGTVSLRSCRASQSVSLSYLHWYQQKPGQAPLLVYGDNSKRPSGIPDRFSGSSSGNTASLTISGVQAEDEADYYCQSSDSSNWVFGGGTKLTVL</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" ref="I7:I11" si="1">LEN(H7)</f>
+        <f t="shared" ref="I7:I9" si="1">LEN(H7)</f>
         <v>231</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1024" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
@@ -884,17 +1973,50 @@
         <v>261</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="3"/>
+    <row r="9" spans="1:1024" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>QVQLVESGGGVVQPGRSLRLSCAASGFTFSSYAMSWVRQAPGKGLEWVSAIWSNGGSTYYADSVKGRFTISRDNAKNSLYLQMNSLRAEDTAVYYCARDYGSYGYFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIVMTQSPLSLPVTPGEPASISCRSSQSLLYSNGNTYLEWYLQKPGQSPQLLIYLVSKLDSGVPDRFSGSGSGTDFTLKISRVEAEDLGIYYCQQSKEVPYTFGAGTKLEIK</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="1"/>
+        <v>247</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(G1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Add m102.3 ipSAE score
</commit_message>
<xml_diff>
--- a/candidates.xlsx
+++ b/candidates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colby/Nipah_gpG_Fv_Generation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E423875A-0961-9941-A230-C954A6166070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F319C840-10C7-DA49-8C27-85FBEE36E58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,16 +21,10 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Antibody Candidates'!$A$1:$V$118</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">'Antibody Candidates'!$V$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Antibody Candidates'!$V$2:$V$128</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Antibody Candidates'!$V$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Antibody Candidates'!$V$2:$V$128</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Antibody Candidates'!$V$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Antibody Candidates'!$V$2:$V$128</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="118" r:id="rId6"/>
+    <pivotCache cacheId="119" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -49,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="578">
   <si>
     <t>antigen_id</t>
   </si>
@@ -1768,6 +1762,21 @@
   </si>
   <si>
     <t>EVQLVESGGGLVKPGGSLKVSCAASGFTFSSYSMVWVRQAPGKGLEWVSRIWSGVDSTGYADSVKGRFTISRDNAKNSLYLQMNSLRAGDTAVYYCARDDDAFDYWGQGTAVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCQASQDIRFYLNWYQQKPGKAPKLLISAASTLQSGVPSRFSGSGSGTDFTLTITSLQPEDFATYYCAGYVPSYTFGPGTKVDIK</t>
+  </si>
+  <si>
+    <t>EIVMTQSPGTPSLSPGERATLSCRASQSIRSTYLAWYQQKPGQAPRLLIYGASSRATGIPDRFSGSGSGTDFTLTISRLEPEDFAVYYCQQYGRSPSFGQGTKVEIK</t>
+  </si>
+  <si>
+    <t>EVQLVQSGAEVKKRGSSVKVSCKSSGGTFSNYAINWVRQAPGQGLEWMGGIIPILGIANYAQKFQGRVTITTDESTSTAYMELSSLRSEDTAVYYCARGWGREQLAPHPSQYYYYYYGMDVWGQGTTVTVSS</t>
+  </si>
+  <si>
+    <t>m102.3</t>
+  </si>
+  <si>
+    <t>6CMI_HL</t>
+  </si>
+  <si>
+    <t>GGGSGGGSGGG</t>
   </si>
 </sst>
 </file>
@@ -1867,7 +1876,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="25">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5718,7 +5741,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{135D55CA-26D1-4FA2-9199-54D547F2C103}" name="PivotTable1" cacheId="118" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{135D55CA-26D1-4FA2-9199-54D547F2C103}" name="PivotTable1" cacheId="119" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A4:C13" firstHeaderRow="0" firstDataRow="0" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="20">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -6462,10 +6485,10 @@
   <dimension ref="A1:V138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B133" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C146" sqref="C146"/>
+      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6595,15 +6618,15 @@
         <v>125</v>
       </c>
       <c r="M2" s="2" t="str">
-        <f>_xlfn.CONCAT(I2,L2,J2)</f>
+        <f t="shared" ref="M2:M33" si="0">_xlfn.CONCAT(I2,L2,J2)</f>
         <v>QVQLVESGGGVVQPGRSLRLSCAASGFTFSSYGMHWVRQAPGKGLEWVAVISYDGSKKYYADSVKGRFTISRDNSKNTLYLQMNSLRAEDTAVYYCARSPFYDSSGYYAMDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQLTQSPSSLSASVGDRVTITCRASQGISSYLAWYQQKPGKAPKLLIYAASTLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQQANSFPPTFGQGTKVEIK</v>
       </c>
       <c r="N2" s="4">
-        <f>LEN(M2)</f>
+        <f t="shared" ref="N2:N33" si="1">LEN(M2)</f>
         <v>246</v>
       </c>
       <c r="O2" s="1" t="b">
-        <f>IF(N2&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" ref="O2:O33" si="2">IF(N2&lt;=250,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="P2" s="1" t="b">
@@ -6663,15 +6686,15 @@
         <v>125</v>
       </c>
       <c r="M3" s="2" t="str">
-        <f>_xlfn.CONCAT(I3,L3,J3)</f>
+        <f t="shared" si="0"/>
         <v>QVQLVESGGGVVQPGKSLRLSCAASGFTFSSYAMSWVRQAPGKGPEWVAFISYDGSNNYYADSVKGRFTISRDNPKNTLYLQMKSLRAEDTAVYYCARWRQRFDMYWGRGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSISSYLNWYQQKPGKAPKLLIYAASSLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQQSYSTPYTFGQGTKVEIK</v>
       </c>
       <c r="N3" s="4">
-        <f>LEN(M3)</f>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="O3" s="1" t="b">
-        <f>IF(N3&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P3" s="1" t="b">
@@ -6731,15 +6754,15 @@
         <v>125</v>
       </c>
       <c r="M4" s="2" t="str">
-        <f>_xlfn.CONCAT(I4,L4,J4)</f>
+        <f t="shared" si="0"/>
         <v>QVQLQESGPGLVKPSETLSLTCTVSGASIRGYYWSWIRQFPGKELEWIGYVYSGSTENYNPSLKSRVTVTLTDTKNSFSLKLNSVTSEDTAVYYCARGGALIYYDVWGTGTTVTVSSGGGSGGGSGGGSGGGSDIQVTQSPVSLSASVGDRVTITCRASQGIDSLNWFQQRPGKAPKLLIYAASQLTGIAPRFRSGSGSGTDFTLTISSLQPEDFATYYCQQYNIYPATFGQGTKVEIK</v>
       </c>
       <c r="N4" s="4">
-        <f>LEN(M4)</f>
+        <f t="shared" si="1"/>
         <v>239</v>
       </c>
       <c r="O4" s="1" t="b">
-        <f>IF(N4&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P4" s="1" t="b">
@@ -6799,15 +6822,15 @@
         <v>125</v>
       </c>
       <c r="M5" s="2" t="str">
-        <f>_xlfn.CONCAT(I5,L5,J5)</f>
+        <f t="shared" si="0"/>
         <v>EVQLVQSGAEVKKPGESLKISCKGSGYTFSYYWIGWVRQMPGKGLEWMGIIYPGDSDTRYSPSFQGQVTISADKSISTAYLQWSSLKASDTAMYYCARGEGVFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSYTLTQAPSVSASGQSVTISCTGTSRDVGTYWYQQIPGRAPKLLIHDKSENQGKTPGIPDRFSGSKSGNTASLVIIRGLQADDEADYYCNSYHGSGSNIFGGGTKLTVD</v>
       </c>
       <c r="N5" s="4">
-        <f>LEN(M5)</f>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="O5" s="1" t="b">
-        <f>IF(N5&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P5" s="1" t="b">
@@ -6867,15 +6890,15 @@
         <v>125</v>
       </c>
       <c r="M6" s="2" t="str">
-        <f>_xlfn.CONCAT(I6,L6,J6)</f>
+        <f t="shared" si="0"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFTFSSYWMNWVRQAPGKGLEWVANINQDGGEKYYVDSVKGRFTISRDNAKNSLYLQMNSLRAEDTAIYYCARDVGGGMDVWGQGTTVTVSSGGGSGGGSGGGSGGGSQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQSSSSLITFGQGTKVEIK</v>
       </c>
       <c r="N6" s="4">
-        <f>LEN(M6)</f>
+        <f t="shared" si="1"/>
         <v>238</v>
       </c>
       <c r="O6" s="1" t="b">
-        <f>IF(N6&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P6" s="1" t="b">
@@ -6931,15 +6954,15 @@
         <v>125</v>
       </c>
       <c r="M7" s="2" t="str">
-        <f>_xlfn.CONCAT(I7,L7,J7)</f>
+        <f t="shared" si="0"/>
         <v>QVQLVESGGGVVQPGRSLRLSCAASGFTFSSYAMSWVRQAPGKGLEWVSAIWSNGGSTYYADSVKGRFTISRDNAKNSLYLQMNSLRAEDTAVYYCARDYGSYGYFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIVMTQSPLSLPVTPGEPASISCRSSQSLLYSNGNTYLEWYLQKPGQSPQLLIYLVSKLDSGVPDRFSGSGSGTDFTLKISRVEAEDLGIYYCQQSKEVPYTFGAGTKLEIK</v>
       </c>
       <c r="N7" s="4">
-        <f>LEN(M7)</f>
+        <f t="shared" si="1"/>
         <v>247</v>
       </c>
       <c r="O7" s="1" t="b">
-        <f>IF(N7&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P7" s="1" t="b">
@@ -7004,15 +7027,15 @@
         <v>125</v>
       </c>
       <c r="M8" s="2" t="str">
-        <f>_xlfn.CONCAT(I8,L8,J8)</f>
+        <f t="shared" si="0"/>
         <v>AVSLVESGGGTVKPGESVTLSCQASGFNFSKYQWVWVRQAPGKGLEWVGQISPDGSKTRYHPSVAGRFTISRDNSNSTLYLHMSNLRPEDTAVYYCGIIPQDNVHGDYSISHWGQGTLLTVSAGGGSGGGSGGGSGGGSAIKLTQSPKSLSASVGDTVTINCTASRPIGDLLSWYKQKPGKPPQLLIYRSSTLASGVSSRYSGSGSDTNFTLTISSLQSSDFATYYCRQTSRFPITFGEGTTINKK</v>
       </c>
       <c r="N8" s="4">
-        <f>LEN(M8)</f>
+        <f t="shared" si="1"/>
         <v>246</v>
       </c>
       <c r="O8" s="1" t="b">
-        <f>IF(N8&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P8" s="1" t="b">
@@ -7077,15 +7100,15 @@
         <v>125</v>
       </c>
       <c r="M9" s="2" t="str">
-        <f>_xlfn.CONCAT(I9,L9,J9)</f>
+        <f t="shared" si="0"/>
         <v>AVSITESGGGTKAPGSSVTLSCKVSGFVFSKYSIAWVRQAPGQGLEWVSQISPDGSTTRYNPAVAGRFTISRDNSNSTAYLQMSNLTPSDTATYYCAIIPQDNEHGDYSLSHWGQGTQLTVSAGGGSGGGSGGGSGGGSAIKLTQSPKSLSAKVGDTVTINCTASAPIGDFLSWYKQKPGQPPQLLIYKSSTLAPGVSSRYSGSGSDTNFTLTISSLQEEDFATYYCQQTATLPITFGEGTTINKK</v>
       </c>
       <c r="N9" s="4">
-        <f>LEN(M9)</f>
+        <f t="shared" si="1"/>
         <v>246</v>
       </c>
       <c r="O9" s="1" t="b">
-        <f>IF(N9&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P9" s="1" t="b">
@@ -7150,15 +7173,15 @@
         <v>125</v>
       </c>
       <c r="M10" s="2" t="str">
-        <f>_xlfn.CONCAT(I10,L10,J10)</f>
+        <f t="shared" si="0"/>
         <v>SISLVESGGGTVAPGSSVTLSCQASGFNFSKYSKAWVRQPPGQPLEWVSRISPDGSTKYYHPDVAGRFTISKDNSKSTVYLAMSNLTAADTATYYCGIIPGDNTHGDYAMSHWGQGTLLTVSAGGGSGGGSGGGSGGGSAITLTQSPSSLSASVGDTVTISCTASRPIGDKLSWYKQKPGQPPQLLIYNASTLAPGVSSRYSGSGSDTSFTLTISSLQEDDFATYYCQQTYTLPITFGQGTTISKK</v>
       </c>
       <c r="N10" s="4">
-        <f>LEN(M10)</f>
+        <f t="shared" si="1"/>
         <v>246</v>
       </c>
       <c r="O10" s="1" t="b">
-        <f>IF(N10&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P10" s="1" t="b">
@@ -7223,15 +7246,15 @@
         <v>125</v>
       </c>
       <c r="M11" s="2" t="str">
-        <f>_xlfn.CONCAT(I11,L11,J11)</f>
+        <f t="shared" si="0"/>
         <v>GVSLTESGGGTVAPGSSVTLSCKASGFNFSKYSHAWVRQAPGQGLTWVGEISPDGSKTRYASSVAGRFTISRDNSNSTVYLQMSSLTPSDTATYYCGIIPGDSVHGERSMSHWGQGTLLTVSAGGGSGGGSGGGSGGGSAITLTQSPSSLSASVGDTVTLNCTASRPIGDRLSWYKQKPGQAPQLLIYRASTLAPGVSSRYSGSGSDTQFTLTISSLQSDDFATYYCQQTSSYPVTFGQGTTITKK</v>
       </c>
       <c r="N11" s="4">
-        <f>LEN(M11)</f>
+        <f t="shared" si="1"/>
         <v>246</v>
       </c>
       <c r="O11" s="1" t="b">
-        <f>IF(N11&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P11" s="1" t="b">
@@ -7296,15 +7319,15 @@
         <v>125</v>
       </c>
       <c r="M12" s="2" t="str">
-        <f>_xlfn.CONCAT(I12,L12,J12)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">EVSLVESGGGTVKPGESVTLSCQASGFNFSKYRLAWVRQPPGQGLVWVSEISPDGTEVKYHPDVKGRFTASRDNSNSTAYLKMNNLQPSDTATYYCGIIPQDSSHGDYSISHWGQGTQLTVSAGGGSGGGSGGGSGGGSTITLTQSPSSLSASVGDTVTINCTASRPIGDFLSWYKQKPGQPPQLLIYRSSTLASGVSSRYSGSGSDTNFTLTISSLQSDDFATYYCQQTYTLPITFGQGTTLTKK </v>
       </c>
       <c r="N12" s="4">
-        <f>LEN(M12)</f>
+        <f t="shared" si="1"/>
         <v>247</v>
       </c>
       <c r="O12" s="1" t="b">
-        <f>IF(N12&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P12" s="1" t="b">
@@ -7363,15 +7386,15 @@
         <v>125</v>
       </c>
       <c r="M13" s="2" t="str">
-        <f>_xlfn.CONCAT(I13,L13,J13)</f>
+        <f t="shared" si="0"/>
         <v>AVSLVESGGGTYAPGSSVTLSCQGSGFNFSKVRKVWVRQPPGGPLEYVAEISPDGSTTTYASSVAGRFTISKDNSNSTLYLSMSNLTPADTATYYCGLIPGDSEHGDRSISHWGQGTLVTVSAGGGSGGGSGGGSGGGSAITLTQSPSSLSASVGDTVTINCTASQPIGNFLSWYKQKPGQPPQLLIYNASTLAPGVSSRYSGSGSDTNFTLTISSLQSEDFATYYCQQTSRLPVTFGQGTTINKK</v>
       </c>
       <c r="N13" s="4">
-        <f>LEN(M13)</f>
+        <f t="shared" si="1"/>
         <v>246</v>
       </c>
       <c r="O13" s="1" t="b">
-        <f>IF(N13&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P13" s="1" t="b">
@@ -7436,15 +7459,15 @@
         <v>125</v>
       </c>
       <c r="M14" s="2" t="str">
-        <f>_xlfn.CONCAT(I14,L14,J14)</f>
+        <f t="shared" si="0"/>
         <v>GISLVESGGGTVKPGESVTLSCKASGFVFSKYSHAWVRQPPGGPLEWVSQISSDGSVTRYASSVSGRFTISRDNSNSTVYLQMNNLRPSDTATYYCGIIPQDNVHGDYAISHWGQGTLLTVTAGGGSGGGSGGGSGGGSAITLTQSPASLSAKVGDTVTLSCTASRPIGDLLSWYKQKPGQPPQLLIYRASTLAPGVDSRYSGSGSDTSFTLTISSLQPEDFATYYCQQTSRFPITFGQGTTIKQA</v>
       </c>
       <c r="N14" s="4">
-        <f>LEN(M14)</f>
+        <f t="shared" si="1"/>
         <v>246</v>
       </c>
       <c r="O14" s="1" t="b">
-        <f>IF(N14&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P14" s="1" t="b">
@@ -7509,15 +7532,15 @@
         <v>125</v>
       </c>
       <c r="M15" s="2" t="str">
-        <f>_xlfn.CONCAT(I15,L15,J15)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">PVSLVESGGGTVAPGSSVTLTCQASGFNFSKYIVAWVRQPPGQPLRFVAMITPDGSKVWLHPEVEGRFTPSKDNSKNTSYLQLKDLQPEDTATYYCGIIPQGSTHGDYSITHWGQGVVLTVTAGGGSGGGSGGGSGGGSMVTLTQSPSSLSASVGDTVTITCTASSPVDNLMSWYQQPPGQPLRLLIYNASTRAPGVSSRFSGSGSDTNFTLTISSLQASDFATYYCQQTYRLPVTFGQGTTLSAA </v>
       </c>
       <c r="N15" s="4">
-        <f>LEN(M15)</f>
+        <f t="shared" si="1"/>
         <v>247</v>
       </c>
       <c r="O15" s="1" t="b">
-        <f>IF(N15&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P15" s="1" t="b">
@@ -7576,15 +7599,15 @@
         <v>125</v>
       </c>
       <c r="M16" s="2" t="str">
-        <f>_xlfn.CONCAT(I16,L16,J16)</f>
+        <f t="shared" si="0"/>
         <v>SIKLTESGGGTVKPGSSVTLSCQASGFNFSKYEVVWVMQKPGQPLQWVGSISPDGSKVRLHPKVKGRFTLSKDNSKNTAYLTMKNLQPEDTATYYCGIIPGGSVHGDRSITHWGQGVELKVVAGGGSGGGSGGGSGGGSMIKLTQSPKSVKAKVGDTVTITCTASEPVDDLVSWYQQKPGQPLRLLIYRSSTLAPGVSSRFSGSGSDTNFTLTISSLQEEDFATYYCMQTSKYPYTFGQGTTLSRA</v>
       </c>
       <c r="N16" s="4">
-        <f>LEN(M16)</f>
+        <f t="shared" si="1"/>
         <v>246</v>
       </c>
       <c r="O16" s="1" t="b">
-        <f>IF(N16&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P16" s="1" t="b">
@@ -7649,15 +7672,15 @@
         <v>125</v>
       </c>
       <c r="M17" s="2" t="str">
-        <f>_xlfn.CONCAT(I17,L17,J17)</f>
+        <f t="shared" si="0"/>
         <v>AITLTESGGGVVAPGSSVTLTCTASGFNFSKYSMVWVRQPPGGPLQWVAQISPDNSTVRYHPAVEGRFTASKDNSKNTAYLAMSDLEPSDTATYYCGIIPQGSTHNDYSIVHWGQGTELRVVAGGGSGGGSGGGSGGGSMIKLTQSPSSLSAKVGDKVTITCTASSPVDNLVSWYKQPPGGPLQLLIYNSSTRAPGVSSRFKGSGSDTNFTLTIESLQEEDFATYYCQQTYKFPITFGQGTKLTRA</v>
       </c>
       <c r="N17" s="4">
-        <f>LEN(M17)</f>
+        <f t="shared" si="1"/>
         <v>246</v>
       </c>
       <c r="O17" s="1" t="b">
-        <f>IF(N17&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P17" s="1" t="b">
@@ -7722,15 +7745,15 @@
         <v>125</v>
       </c>
       <c r="M18" s="2" t="str">
-        <f>_xlfn.CONCAT(I18,L18,J18)</f>
+        <f t="shared" si="0"/>
         <v>SISLTESGGGTVAPGSSVTLTCTASGFNFSKYSVAWVRQPPGQPLQWVALISPDGSKKWYHPDVKGRATISKDNSKNTSYLTLSNLQPSDTATYYCGIIPGGNIHGDYSMTHWGQGTQLTVVAGGGSGGGSGGGSGGGSMITLTQSPLSLSAKVGDTVTITCTASSPVDDLVSWYQQKPGQPLRLLIRNASERAPGVSSRFSGSGSDTTFTLTISSVQEEDFATYYCQQTSKLPYTFGQGTTLSRA</v>
       </c>
       <c r="N18" s="4">
-        <f>LEN(M18)</f>
+        <f t="shared" si="1"/>
         <v>246</v>
       </c>
       <c r="O18" s="1" t="b">
-        <f>IF(N18&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P18" s="1" t="b">
@@ -7795,15 +7818,15 @@
         <v>125</v>
       </c>
       <c r="M19" s="2" t="str">
-        <f>_xlfn.CONCAT(I19,L19,J19)</f>
+        <f t="shared" si="0"/>
         <v>AVTLTESGGGTVAPGSSVTLTCTASGFNFSKYILAWVRQAPGQPLEWVASISPDGSKTRYHPAVKGRATASKDNSKNTAYLELKDLRPEDTATYYCGIIPQGSVHGDYSMTHWGQGTELRVEAGGGSGGGSGGGSGGGSPVVLTQSPLSLSAKVGDTVTITCTASSPVDNLVSWYKQAPGQPLQLLIYNATTRAPGVPSRFTGSGSDTTFTLTISSLQPEDFAVYYCQQTYKFPITFGQGTRLTPA</v>
       </c>
       <c r="N19" s="4">
-        <f>LEN(M19)</f>
+        <f t="shared" si="1"/>
         <v>246</v>
       </c>
       <c r="O19" s="1" t="b">
-        <f>IF(N19&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P19" s="1" t="b">
@@ -7868,15 +7891,15 @@
         <v>125</v>
       </c>
       <c r="M20" s="2" t="str">
-        <f>_xlfn.CONCAT(I20,L20,J20)</f>
+        <f t="shared" si="0"/>
         <v>PVKLVESGGGTVAPGSSVTLTCKASGFNFSKYMVQWVRQAPGGAFQWVGLISPDGSTKWYHPDVEGRFTISKDNSKNTAYLEMRNLTPADTAVYYCGIVPQGSVHGDYSITHWGQGVTLTVTAGGGSGGGSGGGSGGGSVVQLTQSPPELSAKVGEKVTITCTASSPVDNLVSWYQQKPGGAPKLLIYNATTLAPGVPSRFSGSGSDTVFTLTIDSLQAEDFATYYCQQTSRLPFTFGQGTVLRPA</v>
       </c>
       <c r="N20" s="4">
-        <f>LEN(M20)</f>
+        <f t="shared" si="1"/>
         <v>246</v>
       </c>
       <c r="O20" s="1" t="b">
-        <f>IF(N20&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P20" s="1" t="b">
@@ -7941,15 +7964,15 @@
         <v>125</v>
       </c>
       <c r="M21" s="2" t="str">
-        <f>_xlfn.CONCAT(I21,L21,J21)</f>
+        <f t="shared" si="0"/>
         <v>AIKLTESGGGTVKPGSSVTLTCQASGFNFSKYIMAWVRQAPGQPLQWVAQISPDNSVKRYHPEVEGRFTASKDNSKNTAYLEMKNLTPADTATYYCAIIPQGSTQGDYSMVHWGQGVELKVVAGGGSGGGSGGGSGGGSPVVLTQSPASLKAAVGDTVTITCTASAPVDNLVSWYKQAPGQPPQLLIYNASTLAPGVPSRFTGSGSDTSFTLTISSLQEEDFATYYCQETSKFPITFGQGTKLEKK</v>
       </c>
       <c r="N21" s="4">
-        <f>LEN(M21)</f>
+        <f t="shared" si="1"/>
         <v>246</v>
       </c>
       <c r="O21" s="1" t="b">
-        <f>IF(N21&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P21" s="1" t="b">
@@ -8014,15 +8037,15 @@
         <v>125</v>
       </c>
       <c r="M22" s="2" t="str">
-        <f>_xlfn.CONCAT(I22,L22,J22)</f>
+        <f t="shared" si="0"/>
         <v>SIKLTESGGGVVAPGESVTLTCTASGFNFSKYEMAWVRQAPGGPLEFVAVISPDGSTTRYHPRVEGRATISRDNSKNTAYLTLRDLTPADTAVYYCGIIPGGSVHGDRALSHWGQGVRLEVRAGGGSGGGSGGGSGGGSMVTLTQSPSSLSAKVGDKVTISCTASEPVDDLVSWYKQAPGGPPQLLISRASTRAPGVPSRFSGSGSDTNFTLTIESLQSSDFATYYCQQTYKFPDTFGQGTTLSEA</v>
       </c>
       <c r="N22" s="4">
-        <f>LEN(M22)</f>
+        <f t="shared" si="1"/>
         <v>246</v>
       </c>
       <c r="O22" s="1" t="b">
-        <f>IF(N22&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P22" s="1" t="b">
@@ -8087,15 +8110,15 @@
         <v>126</v>
       </c>
       <c r="M23" s="2" t="str">
-        <f>_xlfn.CONCAT(I23,L23,J23)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">SVTLVESGDQTVAPGGSVTLSCTSSGGSFGNSGVSWVKQQPGGPLQWIGGIIPSLGISKVSPEYAGRVTISSDSSNNTAYLTISNLTAADTATYYCALGEGEDVFASSPFASNVNLGALSVWGQGTKVTVSGGGSGGGSGGGSITVTQSPSSPSLKVGETATLTCTLSAPVPRSNVAWYKQQPGQPPTLLIYGGSTRAPGVPSRYSGSGSGTTFTLTITALKPEDFATYYCQVYGENPSFGQGTTLKLK </v>
       </c>
       <c r="N23" s="4">
-        <f>LEN(M23)</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
       <c r="O23" s="1" t="b">
-        <f>IF(N23&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P23" s="1" t="b">
@@ -8154,15 +8177,15 @@
         <v>126</v>
       </c>
       <c r="M24" s="2" t="str">
-        <f>_xlfn.CONCAT(I24,L24,J24)</f>
+        <f t="shared" si="0"/>
         <v>GVKLVQSGDLTVKPGGSVTLSCKSEGGSFGNSSVAWVRQRPGGPYEYIGSIIPAYGVSRVSPEYEGRVTISADVANNTAYLTISNLTPEDTATYYCALGPGEVVYAASPFDEKLLTGALSVWGEGTLVTVTGGGSGGGSGGGSITVTQSPSSPSLSVGDTATLTCTLSSSVATSNVAWYKQLPGQPPELLISGGSTRAPGVPSRYSGSGSGTTFTLTISSLQASDFATYYCQVYGENPSFGQGTTLTLK</v>
       </c>
       <c r="N24" s="4">
-        <f>LEN(M24)</f>
+        <f t="shared" si="1"/>
         <v>249</v>
       </c>
       <c r="O24" s="1" t="b">
-        <f>IF(N24&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P24" s="1" t="b">
@@ -8227,15 +8250,15 @@
         <v>126</v>
       </c>
       <c r="M25" s="2" t="str">
-        <f>_xlfn.CONCAT(I25,L25,J25)</f>
+        <f t="shared" si="0"/>
         <v>AVKLVQSGDQTVAPGGSVTLSCTSSGGSFGNSSVAWVRQRPGGPFEFIGSIIPSLGISRYNSKYKGRVTISSDAANNTAYLTISNLTAADTATYYCALGPGESVFASHPFKEKLLTGALSVWGEGTLVTVSGGGSGGGSGGGSITVTQSPSSPSKSVGDTVTLTCTLSSSVPVSQVAWYKQHPGQPPELLIYGGSTRASGVPSRYSGSGSGTTFTLTISSLQPEDFATYYCQVYGEEPSFGQGTTVTLA</v>
       </c>
       <c r="N25" s="4">
-        <f>LEN(M25)</f>
+        <f t="shared" si="1"/>
         <v>249</v>
       </c>
       <c r="O25" s="1" t="b">
-        <f>IF(N25&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P25" s="1" t="b">
@@ -8300,15 +8323,15 @@
         <v>126</v>
       </c>
       <c r="M26" s="2" t="str">
-        <f>_xlfn.CONCAT(I26,L26,J26)</f>
+        <f t="shared" si="0"/>
         <v>SITLVQSGDVTVAPGGSVTLTCTSSGGSFGNKAVAWVRQRPGGPYEWLGFIIPAYGVSRYNPAYEGRVTISVDSASNTASLTISNLTAADTATYYCALGEGEIVYAASPFDENYKLGALYIWGQGTKVTVSGGGSGGGSGGGSITLTQSPSSPSLSVGETATLTCTASAPVPKSNVAWYKQLPGQPPELLIYGGSTRASGVPSRYSGSGSGTTFTLTISSLTADDFATYYCQVYGENPSFGEGTTLTLK</v>
       </c>
       <c r="N26" s="4">
-        <f>LEN(M26)</f>
+        <f t="shared" si="1"/>
         <v>249</v>
       </c>
       <c r="O26" s="1" t="b">
-        <f>IF(N26&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P26" s="1" t="b">
@@ -8373,15 +8396,15 @@
         <v>126</v>
       </c>
       <c r="M27" s="2" t="str">
-        <f>_xlfn.CONCAT(I27,L27,J27)</f>
+        <f t="shared" si="0"/>
         <v>SVTLVQSGDQTVPIGGSVTLSCTANGGSFGNKGVAWVRQRPGGPYEFLGFIKPAIGESRYHPKYKGRVTISSDVSSNTAYLTISNLTPEDTAVYYCALGEAEDVFAAHPFKTDLLLGALSIWGQGTRVTVTGGGSGGGSGGGSITVTQSPSSPSLSVGETAVLTCTLSQPVPQSQVAWYKQLPGQPPTLLISGGSTRASGVPSRYSGSGSGTTFTLTISSLLPEDFATYYCQVVGKEPSFGQGTTLTLK</v>
       </c>
       <c r="N27" s="4">
-        <f>LEN(M27)</f>
+        <f t="shared" si="1"/>
         <v>249</v>
       </c>
       <c r="O27" s="1" t="b">
-        <f>IF(N27&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P27" s="1" t="b">
@@ -8446,15 +8469,15 @@
         <v>126</v>
       </c>
       <c r="M28" s="2" t="str">
-        <f>_xlfn.CONCAT(I28,L28,J28)</f>
+        <f t="shared" si="0"/>
         <v>SVKLVQSGDQTVPVGGSVTLSCTASGGSFGNYGVAWVRQRPGGPLEYIGSIIPAYGISTVNPKYEGRVTISADPTNNTAYLTISNLTPEDTATYYCALGPGEVVFASSPFDIDVLTGALWVWGEGTKVTVTGGGSGGGSGGGSITVTQSPSSPSLKVGETATLTCTLSAPVAKSNVAWYKQLPGQPPELLIYGGSTRASGVPSRYSGSGSGTTFTLTISSLQPEDFATYYCQVVGKNPSFGQGTLLKLK</v>
       </c>
       <c r="N28" s="4">
-        <f>LEN(M28)</f>
+        <f t="shared" si="1"/>
         <v>249</v>
       </c>
       <c r="O28" s="1" t="b">
-        <f>IF(N28&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P28" s="1" t="b">
@@ -8519,15 +8542,15 @@
         <v>126</v>
       </c>
       <c r="M29" s="2" t="str">
-        <f>_xlfn.CONCAT(I29,L29,J29)</f>
+        <f t="shared" si="0"/>
         <v>SISLVQSSDQTVAPGGSVTLSCTSSGGSFGNSGVAWVRQAPGGPPVYIGGIIPATGVSTYNAAFKGRVTISSDSSNNTAYLTISGLTAADTATYYCALGPAENVFASHPFAEDVNLGALSVWGQGTLVTVTGGGSGGGSGGGSITVTESPSSPELSVGETAVLSCTLSSSVPQSNVAWYKQKPGQPPELLIYGGSTRASGVPSRYSGSGSGTTFYLTISSLEPEDFATYYCQVYGTSPSFGQGTTLKLK</v>
       </c>
       <c r="N29" s="4">
-        <f>LEN(M29)</f>
+        <f t="shared" si="1"/>
         <v>249</v>
       </c>
       <c r="O29" s="1" t="b">
-        <f>IF(N29&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P29" s="1" t="b">
@@ -8592,15 +8615,15 @@
         <v>126</v>
       </c>
       <c r="M30" s="2" t="str">
-        <f>_xlfn.CONCAT(I30,L30,J30)</f>
+        <f t="shared" si="0"/>
         <v>AVSLVESGDQTVAPGGSVTLSCTSSGGSFGNSGVAWVRQAPGGPLEFLGFIIPALGVSKVNSKYEGRVTISSDPANNTAYLTISNLTAADTATYYCGLGTGESVFASSPFDEKLLLGALSVWGQGTKVTVTGGGSGGGSGGGSITVTQSPASPEKKVGETATLTCTLSSAVPKSNVAWYKQKPGQPPELLIYGGSTRASGVPSRYSGSGSGTTFYLTISSLQPEDFATYYCRVYGEEPSFGQGTTLKLK</v>
       </c>
       <c r="N30" s="4">
-        <f>LEN(M30)</f>
+        <f t="shared" si="1"/>
         <v>249</v>
       </c>
       <c r="O30" s="1" t="b">
-        <f>IF(N30&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P30" s="1" t="b">
@@ -8659,15 +8682,15 @@
         <v>125</v>
       </c>
       <c r="M31" s="2" t="str">
-        <f>_xlfn.CONCAT(I31,L31,J31)</f>
+        <f t="shared" si="0"/>
         <v>VQLQESGPGLVKPSQSLSLTCTVTGYSITTGYAWNWIRQFPGNKLEWMGYISYSGSTYYPSLKSRISITRDTSKNQFFLQLSIVTTEDTATYYCARGTTLPDYVDFWGQGTSVTVSSGGGSGGGSGGGSGGGSDIQLTQSPSSLSASVGDRVTITCRASQTISTYLNWYQQKPGKAPKLLIYAASTLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYFCLQHFWTPPITFGQGTRLEIK</v>
       </c>
       <c r="N31" s="4">
-        <f>LEN(M31)</f>
+        <f t="shared" si="1"/>
         <v>241</v>
       </c>
       <c r="O31" s="1" t="b">
-        <f>IF(N31&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P31" s="1" t="b">
@@ -8718,15 +8741,15 @@
         <v>126</v>
       </c>
       <c r="M32" s="2" t="str">
-        <f>_xlfn.CONCAT(I32,L32,J32)</f>
+        <f t="shared" si="0"/>
         <v>QVQLQESGPGLVKPSETLSVTCTVSGGSIGSNNYWSWIRQPAGKGLEWIGYIYYSGSTNYNPSLKSRVTMSVDTSKNQFSLKLSSVTAADTAVYYCVRNYYDSSDSSGYYFMDVWGQGTTVTVSSGGGSGGGSGGGSDIVMTQSPLSLSVTPGEPASISCRSSQSLLHSNGYNYLDWYLQKPGQSPQLLIYLGSNRASGVPDRFSGSGSGTDFTLKISRVEAEDVGVYYCMQALQTPTFGQGTRLEIK</v>
       </c>
       <c r="N32" s="4">
-        <f>LEN(M32)</f>
+        <f t="shared" si="1"/>
         <v>248</v>
       </c>
       <c r="O32" s="1" t="b">
-        <f>IF(N32&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P32" s="1" t="b">
@@ -8777,15 +8800,15 @@
         <v>125</v>
       </c>
       <c r="M33" s="2" t="str">
-        <f>_xlfn.CONCAT(I33,L33,J33)</f>
+        <f t="shared" si="0"/>
         <v>QVQLVQSGAEVKKPGESLKISCKGSGYRFSSYWIGWVRQMPGKGLEWMGIIYPGDSDTRYSPSFQGQVTISADKSISTAYLQWSSLKASDTAMYYCARQGPDYYYGMDVWGQGTTVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSTLSASVGDRVTITCRASQSISSWLAWYQQKPGKAPKLLIYKASELQSGVPSRFSGSGSGTEFTLTISSLQPDDFATYYCQQYINSYTFGQGTKVEIK</v>
       </c>
       <c r="N33" s="4">
-        <f>LEN(M33)</f>
+        <f t="shared" si="1"/>
         <v>242</v>
       </c>
       <c r="O33" s="1" t="b">
-        <f>IF(N33&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P33" s="1" t="b">
@@ -8836,15 +8859,15 @@
         <v>125</v>
       </c>
       <c r="M34" s="2" t="str">
-        <f>_xlfn.CONCAT(I34,L34,J34)</f>
+        <f t="shared" ref="M34:M65" si="3">_xlfn.CONCAT(I34,L34,J34)</f>
         <v>QVQLQQSGPELVKPGASVKLSCKASGYTFTDYYMHWVKQRPGQGLEWIGEINPNSGGTNTYDQKFKGRATLTVDKSSSTAYLQLSSLTSEDSAVYYCARSPPWYFDYWGQGTTLTVSGGGSGGGSGGGSGGGSDIVMTQSPSSMFASVGETVTITCRASENIYSNLAWYQQKPGQSPKLLIYWASTRHTGVPDRFTGSGSGTDFTLTISSVQAEDLALYYCQHYGSYSFTFGSGTKLEIK</v>
       </c>
       <c r="N34" s="4">
-        <f>LEN(M34)</f>
+        <f t="shared" ref="N34:N65" si="4">LEN(M34)</f>
         <v>240</v>
       </c>
       <c r="O34" s="1" t="b">
-        <f>IF(N34&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" ref="O34:O65" si="5">IF(N34&lt;=250,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="P34" s="1" t="b">
@@ -8895,15 +8918,15 @@
         <v>125</v>
       </c>
       <c r="M35" s="2" t="str">
-        <f>_xlfn.CONCAT(I35,L35,J35)</f>
+        <f t="shared" si="3"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVSYSSIHWVRQAPGKGLEWVASISSYYGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARSRNYVYSSGYLDFWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQSSYSSPPTFGQGTKVEIK</v>
       </c>
       <c r="N35" s="4">
-        <f>LEN(M35)</f>
+        <f t="shared" si="4"/>
         <v>246</v>
       </c>
       <c r="O35" s="1" t="b">
-        <f>IF(N35&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P35" s="1" t="b">
@@ -8954,15 +8977,15 @@
         <v>125</v>
       </c>
       <c r="M36" s="2" t="str">
-        <f>_xlfn.CONCAT(I36,L36,J36)</f>
+        <f t="shared" si="3"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNIYYSSIHWVRQAPGKGLEWVASISPYYGSTSYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARDYGHYYYAMDYWGQGTLVTVSSGGGSGGGSGGGSGGGSEIVMTQSPATLSVSPGERATLSCRASQSVSSYLAWYQQKPGQAPRLLIYGASTRATGIPARFSGSGSGTEFTLTISSLQSEDSAVYYCQQYNNWPPITFGQGTRLEIK</v>
       </c>
       <c r="N36" s="4">
-        <f>LEN(M36)</f>
+        <f t="shared" si="4"/>
         <v>244</v>
       </c>
       <c r="O36" s="1" t="b">
-        <f>IF(N36&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P36" s="1" t="b">
@@ -9013,15 +9036,15 @@
         <v>126</v>
       </c>
       <c r="M37" s="2" t="str">
-        <f>_xlfn.CONCAT(I37,L37,J37)</f>
+        <f t="shared" si="3"/>
         <v>QVQLQESGPGLVKPSETLSLSCVVSGDSSSTNYYWGWIRQPPGKGLEWIGYIYGSGDTAYNPSLKSRVTISVDTSKNQFSLKLSSVTAADTAVYYCARRSWGYGYNGYSTYYYYYYFDQGYFDVWGPGTLVTGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSIGSYLNWYQQKPGKAPKLLIYAASTLQSGVPSRFSGSGSGTEFTLTISSLQPEDFATYYCQQSYSWGQGTKVEIK</v>
       </c>
       <c r="N37" s="4">
-        <f>LEN(M37)</f>
+        <f t="shared" si="4"/>
         <v>247</v>
       </c>
       <c r="O37" s="1" t="b">
-        <f>IF(N37&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P37" s="1" t="b">
@@ -9072,15 +9095,15 @@
         <v>125</v>
       </c>
       <c r="M38" s="2" t="str">
-        <f>_xlfn.CONCAT(I38,L38,J38)</f>
+        <f t="shared" si="3"/>
         <v>QVQLVQSGAEVKKPGASVKVSCKASGYTFTSYGISWVRQAPGQGLEWMGWISAHNGDTNYAQKFQGRVTMTRDTSITTAYMELRSDDTAVYYCARDGSVGGFYWGQGTLVTVSSGGGSGGGSGGGSGGGSEIVLTQSPGTLSLSPGERATLSCRASQSVSSYLAWYQQKPGQAPRLLIYGASSRATGIPDRFSGSGSGTDFTLTISRLEPEDFAVYYCQQYGSSPITFGQGTRLEIK</v>
       </c>
       <c r="N38" s="4">
-        <f>LEN(M38)</f>
+        <f t="shared" si="4"/>
         <v>237</v>
       </c>
       <c r="O38" s="1" t="b">
-        <f>IF(N38&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P38" s="1" t="b">
@@ -9131,15 +9154,15 @@
         <v>125</v>
       </c>
       <c r="M39" s="2" t="str">
-        <f>_xlfn.CONCAT(I39,L39,J39)</f>
+        <f t="shared" si="3"/>
         <v>EVQLLESGGGLVQPGGSLRLSCAASGFNVSYSSIHWVRQAPGKGLEWVASISPYYGSTSYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARSYYWYWSGWGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQSYGSPPTFGQGTKVEIK</v>
       </c>
       <c r="N39" s="4">
-        <f>LEN(M39)</f>
+        <f t="shared" si="4"/>
         <v>238</v>
       </c>
       <c r="O39" s="1" t="b">
-        <f>IF(N39&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P39" s="1" t="b">
@@ -9190,15 +9213,15 @@
         <v>125</v>
       </c>
       <c r="M40" s="2" t="str">
-        <f>_xlfn.CONCAT(I40,L40,J40)</f>
+        <f t="shared" si="3"/>
         <v>QVQLQESGPGLVKPSQTLSLTCTVSGGSISSGHYAWWIRQPPGKGLEWIACIYSSSGSTYYNPSLKSRITISVDTSKNQFSLKLSSVTAADTAVYYCARRQRGYDYDYYYGMDVWGQGTTVTVSSGGGSGGGSGGGSGGGSDIQLTQSPSSLSASVGDRVTITCRASQGISRNLAWYQQKPGKAPKLLIYAASSLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQQSNNWPITFGQGTKVEIK</v>
       </c>
       <c r="N40" s="4">
-        <f>LEN(M40)</f>
+        <f t="shared" si="4"/>
         <v>248</v>
       </c>
       <c r="O40" s="1" t="b">
-        <f>IF(N40&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P40" s="1" t="b">
@@ -9249,15 +9272,15 @@
         <v>125</v>
       </c>
       <c r="M41" s="2" t="str">
-        <f>_xlfn.CONCAT(I41,L41,J41)</f>
+        <f t="shared" si="3"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNIYYSSIHWVRQAPGKGLEWVASIYSYYSSTSYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARVYGYLSYSYFYWGLDVWGQGTLVTVSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEI</v>
       </c>
       <c r="N41" s="4">
-        <f>LEN(M41)</f>
+        <f t="shared" si="4"/>
         <v>246</v>
       </c>
       <c r="O41" s="1" t="b">
-        <f>IF(N41&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P41" s="1" t="b">
@@ -9308,15 +9331,15 @@
         <v>125</v>
       </c>
       <c r="M42" s="2" t="str">
-        <f>_xlfn.CONCAT(I42,L42,J42)</f>
+        <f t="shared" si="3"/>
         <v>EVQLQQSGAELVKPGASVKLSCTASGFNIKDTYVHWVKQRPEQGLEWIGRIDPANGYTKYDPKFQGKATITADTSSNTAYLQLSSLTSEDTAVYYCVRPLYDYYAMDYWGQGTTLTVSSGGGSGGGSGGGSGGGSDIVMTQSPSSLAMSAGRVSITCRTSQSISSYLNWVQQKPGKSPKLLIYWASTRESGVPDRFTGSGSGTDFTLTISRVEAEDLGVYYCMQGTHVPYTFGGGTKLEIK</v>
       </c>
       <c r="N42" s="4">
-        <f>LEN(M42)</f>
+        <f t="shared" si="4"/>
         <v>241</v>
       </c>
       <c r="O42" s="1" t="b">
-        <f>IF(N42&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P42" s="1" t="b">
@@ -9367,15 +9390,15 @@
         <v>125</v>
       </c>
       <c r="M43" s="2" t="str">
-        <f>_xlfn.CONCAT(I43,L43,J43)</f>
+        <f t="shared" si="3"/>
         <v>EVQLVESGGGLVKPGGSLRLSCAASGFTFSSYAMHWVRQAPGKGLEWVSAISGGGGSTYYADSVKGRFTISRDNSKNTLYLQMRAEDTAVYYCAKDDADWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPFTFGQGTKVEIK</v>
       </c>
       <c r="N43" s="4">
-        <f>LEN(M43)</f>
+        <f t="shared" si="4"/>
         <v>233</v>
       </c>
       <c r="O43" s="1" t="b">
-        <f>IF(N43&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P43" s="1" t="b">
@@ -9426,15 +9449,15 @@
         <v>125</v>
       </c>
       <c r="M44" s="2" t="str">
-        <f>_xlfn.CONCAT(I44,L44,J44)</f>
+        <f t="shared" si="3"/>
         <v>QVQLQESGPGLVKPSQTLSLTCTVSGGSISSGSYYWIRQSPGKGLEWIGYIYYSGSTNYNPSLKSRVTISVDTSKNQFSLKLSSVTAADTAVYYCARHRYYDRGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPASLSASVGETVTITCRASENIYSNLAWYQQKQGKSPQLLVYAATDLADGVPSRFSGSGSGTQFSLKINSLQPEDFGSYYCQHFWDTPWTFGQGTRVE</v>
       </c>
       <c r="N44" s="4">
-        <f>LEN(M44)</f>
+        <f t="shared" si="4"/>
         <v>234</v>
       </c>
       <c r="O44" s="1" t="b">
-        <f>IF(N44&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P44" s="1" t="b">
@@ -9485,15 +9508,15 @@
         <v>125</v>
       </c>
       <c r="M45" s="2" t="str">
-        <f>_xlfn.CONCAT(I45,L45,J45)</f>
+        <f t="shared" si="3"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNLYSSSIHWVRQAPGKGLEWVAYISSSGTHYADSVKGRFTISADTSKNTAYLQMRAEDTAVYYCARVGHYYSSGGYYYAMDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYSSYWTFGQGTKVEIK</v>
       </c>
       <c r="N45" s="4">
-        <f>LEN(M45)</f>
+        <f t="shared" si="4"/>
         <v>242</v>
       </c>
       <c r="O45" s="1" t="b">
-        <f>IF(N45&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P45" s="1" t="b">
@@ -9544,15 +9567,15 @@
         <v>126</v>
       </c>
       <c r="M46" s="2" t="str">
-        <f>_xlfn.CONCAT(I46,L46,J46)</f>
+        <f t="shared" si="3"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVVDSGISWVRQAPGKGLEWVSYISSSSGSTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARAHYYGSYFGSVVYYYGLDVWGQGTLVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYDTYPITFGQGTKVEIK</v>
       </c>
       <c r="N46" s="4">
-        <f>LEN(M46)</f>
+        <f t="shared" si="4"/>
         <v>247</v>
       </c>
       <c r="O46" s="1" t="b">
-        <f>IF(N46&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P46" s="1" t="b">
@@ -9603,15 +9626,15 @@
         <v>125</v>
       </c>
       <c r="M47" s="2" t="str">
-        <f>_xlfn.CONCAT(I47,L47,J47)</f>
+        <f t="shared" si="3"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVYSSSIHWVRQAPGKGLEWVASISSYYGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARSYSTYYYGYWYFDVWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSAAVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYNYYWLITFGQGTKVEIK</v>
       </c>
       <c r="N47" s="4">
-        <f>LEN(M47)</f>
+        <f t="shared" si="4"/>
         <v>247</v>
       </c>
       <c r="O47" s="1" t="b">
-        <f>IF(N47&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P47" s="1" t="b">
@@ -9662,15 +9685,15 @@
         <v>125</v>
       </c>
       <c r="M48" s="2" t="str">
-        <f>_xlfn.CONCAT(I48,L48,J48)</f>
+        <f t="shared" si="3"/>
         <v>QVQLQQPGAELVKPGASVKLSCKASGYTFTSDWIHWVKQRPGHGLEWIGEIIPSYGRANYNEKIQKKATLTADKSSSTAFMHLSSLTSEDSAVYYCARERGDGYFAVWGAGTTVTVSSGGGSGGGSGGGSGGGSDILLTQSPAILSVSPGERVSFSCRASQSIGTDIHWYQQRTNGSPRLLIKYASESISGIPSRFSGSGSGTDFTLSINSVESEDIANYYCQQSNRWPFTFGSGTKLEIK</v>
       </c>
       <c r="N48" s="4">
-        <f>LEN(M48)</f>
+        <f t="shared" si="4"/>
         <v>241</v>
       </c>
       <c r="O48" s="1" t="b">
-        <f>IF(N48&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P48" s="1" t="b">
@@ -9721,15 +9744,15 @@
         <v>125</v>
       </c>
       <c r="M49" s="2" t="str">
-        <f>_xlfn.CONCAT(I49,L49,J49)</f>
+        <f t="shared" si="3"/>
         <v>VRLLESGGGLVQPGGSLKLSCAASGFDYSRYWMSWVRQAPGKGLKWIGEINPVSSTINYTPSLKDKFIISRDNAKDTLYLQISKVRSEDTALYYCARLYYGYGYWYFDVWGAGTTVTVSSGGGSGGGSGGGSGGGSDIVLTQSPAIMSAAPGDKVTMTCSASSSVSYIHWYQQKSGTSPKRWIYDTSKLTSGVPVRFSGSGSGTSYSLTINTMEAEDAATYYCQQWSSHPQTFGGGTKLEIl</v>
       </c>
       <c r="N49" s="4">
-        <f>LEN(M49)</f>
+        <f t="shared" si="4"/>
         <v>242</v>
       </c>
       <c r="O49" s="1" t="b">
-        <f>IF(N49&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P49" s="1" t="b">
@@ -9780,15 +9803,15 @@
         <v>125</v>
       </c>
       <c r="M50" s="2" t="str">
-        <f>_xlfn.CONCAT(I50,L50,J50)</f>
+        <f t="shared" si="3"/>
         <v>QVQLQESGPGLVQPSQSLSLTCTVSGFSLTSYGVHWVRQSPGKGLEWLGVIWAGGSTDYNSALKSRLSISRDTSKNQVFLKMNSLQTDDTAMYYCAKHGSSNGDYWGQGTSVTVSSGGGSGGGSGGGSGGGSDIVMTQSPDSLAVSLGERATINCKSSQSVLYSSNNKNYLAWYQQKPEGQPPNLLIYWASTRESGVPDRFSGSGSGTDFTLTISSLQAEDVAVYYCQQYYSAPTFGQGTKLEIK</v>
       </c>
       <c r="N50" s="4">
-        <f>LEN(M50)</f>
+        <f t="shared" si="4"/>
         <v>245</v>
       </c>
       <c r="O50" s="1" t="b">
-        <f>IF(N50&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P50" s="1" t="b">
@@ -9839,15 +9862,15 @@
         <v>125</v>
       </c>
       <c r="M51" s="2" t="str">
-        <f>_xlfn.CONCAT(I51,L51,J51)</f>
+        <f t="shared" si="3"/>
         <v>QVQLQESGPGLVKPSETLSLTCTVSGGSVSSGGYFWSWIRQPPGKGLEWIGCIYYSGSTNYNPSLKSRVTISVDTSKNQFSLKLSSVTAADTAVYYCARVDSFYYGMDVWGQGTTVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQGIRNDLGWYQQKPGKAPKLLIYAASSLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQQSYSTPRTFGQGTKVEIK</v>
       </c>
       <c r="N51" s="4">
-        <f>LEN(M51)</f>
+        <f t="shared" si="4"/>
         <v>243</v>
       </c>
       <c r="O51" s="1" t="b">
-        <f>IF(N51&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P51" s="1" t="b">
@@ -9898,15 +9921,15 @@
         <v>125</v>
       </c>
       <c r="M52" s="2" t="str">
-        <f>_xlfn.CONCAT(I52,L52,J52)</f>
+        <f t="shared" si="3"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFTFSSYAMSWVRQAPGKGLEWVSAISGSGGSTYYADSVKGRFTISRDNSKNTLYLQMNSLRAEDTAVYYCARQVWFGGFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N52" s="4">
-        <f>LEN(M52)</f>
+        <f t="shared" si="4"/>
         <v>241</v>
       </c>
       <c r="O52" s="1" t="b">
-        <f>IF(N52&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P52" s="1" t="b">
@@ -9957,15 +9980,15 @@
         <v>125</v>
       </c>
       <c r="M53" s="2" t="str">
-        <f>_xlfn.CONCAT(I53,L53,J53)</f>
+        <f t="shared" si="3"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVSSSYIHWVRQAPGKGLEWVASISSYYGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARSRQFWYSGLDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N53" s="4">
-        <f>LEN(M53)</f>
+        <f t="shared" si="4"/>
         <v>243</v>
       </c>
       <c r="O53" s="1" t="b">
-        <f>IF(N53&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P53" s="1" t="b">
@@ -10016,15 +10039,15 @@
         <v>125</v>
       </c>
       <c r="M54" s="2" t="str">
-        <f>_xlfn.CONCAT(I54,L54,J54)</f>
+        <f t="shared" si="3"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNISSSSIHWVRQAPGKGLEWVASIYSYSGYTSYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARGGSSYFGYYAMDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N54" s="4">
-        <f>LEN(M54)</f>
+        <f t="shared" si="4"/>
         <v>245</v>
       </c>
       <c r="O54" s="1" t="b">
-        <f>IF(N54&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P54" s="1" t="b">
@@ -10075,15 +10098,15 @@
         <v>125</v>
       </c>
       <c r="M55" s="2" t="str">
-        <f>_xlfn.CONCAT(I55,L55,J55)</f>
+        <f t="shared" si="3"/>
         <v>QVQLVQSGAEVKKPGSSVKVSCKASGGTFSSYSISWVRQAPGQGLEWMGGIIIFGTANYAQKFQGRVTITADESTSTAYMELSSLRSEDTAVYYCARGQGTLVDFYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSISSYLNWYQQKPGKAPKLLIYAASSLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQQSYSTPRTFGQGTKVEIK</v>
       </c>
       <c r="N55" s="4">
-        <f>LEN(M55)</f>
+        <f t="shared" si="4"/>
         <v>240</v>
       </c>
       <c r="O55" s="1" t="b">
-        <f>IF(N55&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P55" s="1" t="b">
@@ -10131,15 +10154,15 @@
         <v>125</v>
       </c>
       <c r="M56" s="2" t="str">
-        <f>_xlfn.CONCAT(I56,L56,J56)</f>
+        <f t="shared" si="3"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVSYYSIHWVRQAPGKGLEWVASIYPYSGYTNYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARYYGYGYWGYAMDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N56" s="4">
-        <f>LEN(M56)</f>
+        <f t="shared" si="4"/>
         <v>245</v>
       </c>
       <c r="O56" s="1" t="b">
-        <f>IF(N56&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P56" s="1" t="b">
@@ -10190,15 +10213,15 @@
         <v>125</v>
       </c>
       <c r="M57" s="2" t="str">
-        <f>_xlfn.CONCAT(I57,L57,J57)</f>
+        <f t="shared" si="3"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFTFSSYAMSWVRQAPGKGLEWVSAISGSGGSTYYADSVKGRFTISRDNSKNTLYLQMNSLRAEDTAVYYCARGYQVYFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N57" s="4">
-        <f>LEN(M57)</f>
+        <f t="shared" si="4"/>
         <v>240</v>
       </c>
       <c r="O57" s="1" t="b">
-        <f>IF(N57&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P57" s="1" t="b">
@@ -10246,15 +10269,15 @@
         <v>125</v>
       </c>
       <c r="M58" s="2" t="str">
-        <f>_xlfn.CONCAT(I58,L58,J58)</f>
+        <f t="shared" si="3"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVSSSYIHWVRQAPGKGLEWVASISSYYGSTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARGWSYSWSYSWSYSGLDVWGQGTTVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQSSSSLITFGQGTKVEIK</v>
       </c>
       <c r="N58" s="4">
-        <f>LEN(M58)</f>
+        <f t="shared" si="4"/>
         <v>249</v>
       </c>
       <c r="O58" s="1" t="b">
-        <f>IF(N58&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P58" s="1" t="b">
@@ -10305,15 +10328,15 @@
         <v>125</v>
       </c>
       <c r="M59" s="2" t="str">
-        <f>_xlfn.CONCAT(I59,L59,J59)</f>
+        <f t="shared" si="3"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNISSSSIHWVRQAPGKGLEWVASIYSYSGYTSYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARGWYYGSSYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N59" s="4">
-        <f>LEN(M59)</f>
+        <f t="shared" si="4"/>
         <v>240</v>
       </c>
       <c r="O59" s="1" t="b">
-        <f>IF(N59&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P59" s="1" t="b">
@@ -10359,15 +10382,15 @@
         <v>125</v>
       </c>
       <c r="M60" s="2" t="str">
-        <f>_xlfn.CONCAT(I60,L60,J60)</f>
+        <f t="shared" si="3"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVSSSYIHWVRQAPGKGLEWVASISSYYGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARYYGTYYGSSYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N60" s="4">
-        <f>LEN(M60)</f>
+        <f t="shared" si="4"/>
         <v>242</v>
       </c>
       <c r="O60" s="1" t="b">
-        <f>IF(N60&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P60" s="1" t="b">
@@ -10413,15 +10436,15 @@
         <v>125</v>
       </c>
       <c r="M61" s="2" t="str">
-        <f>_xlfn.CONCAT(I61,L61,J61)</f>
+        <f t="shared" si="3"/>
         <v>QMQLVQSGAEVKKPGESLKISCKGSGYSFTSYWIGWVRQMPGKGLEWMGIIYPGDSDTRYSPSFQGQVTISADKSISTAYLQWSSLKASDTAIYYCARHYYGGQYFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQGIRNDLGWYQQKPGKAPKLLIYAASSLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQQSYSTPYTFGQGTKLEIK</v>
       </c>
       <c r="N61" s="4">
-        <f>LEN(M61)</f>
+        <f t="shared" si="4"/>
         <v>242</v>
       </c>
       <c r="O61" s="1" t="b">
-        <f>IF(N61&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P61" s="1" t="b">
@@ -10472,15 +10495,15 @@
         <v>125</v>
       </c>
       <c r="M62" s="2" t="str">
-        <f>_xlfn.CONCAT(I62,L62,J62)</f>
+        <f t="shared" si="3"/>
         <v>QVQLVQSGAEVKKPGSSVKVSCKASGGTFSSYAISWVRQAPGQGLEWMGGIIPIFGTANYAQKFQGRVTITADESTSTAYMELSSLRSEDTAVYYCARWYDGYFVYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSISSYLNWYQQKPGKAPKLLIYAASSLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQQSYSTPYTFGQGTKVEIK</v>
       </c>
       <c r="N62" s="4">
-        <f>LEN(M62)</f>
+        <f t="shared" si="4"/>
         <v>240</v>
       </c>
       <c r="O62" s="1" t="b">
-        <f>IF(N62&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P62" s="1" t="b">
@@ -10531,15 +10554,15 @@
         <v>125</v>
       </c>
       <c r="M63" s="2" t="str">
-        <f>_xlfn.CONCAT(I63,L63,J63)</f>
+        <f t="shared" si="3"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVSSSSIHWVRQAPGKGLEWVASISSYYGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARSRQFWYSGLDYWGQGTLVTVFNGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N63" s="4">
-        <f>LEN(M63)</f>
+        <f t="shared" si="4"/>
         <v>243</v>
       </c>
       <c r="O63" s="1" t="b">
-        <f>IF(N63&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P63" s="1" t="b">
@@ -10590,15 +10613,15 @@
         <v>125</v>
       </c>
       <c r="M64" s="2" t="str">
-        <f>_xlfn.CONCAT(I64,L64,J64)</f>
+        <f t="shared" si="3"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNISSSSIHWVRQAPGKGLEWVASIYSYYGSTYYADSVKGRFTISADTSKNTAYLQMRAEDTAVYYCARGWRSYAMDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQSSSSLITFGQGTKVEIK</v>
       </c>
       <c r="N64" s="4">
-        <f>LEN(M64)</f>
+        <f t="shared" si="4"/>
         <v>238</v>
       </c>
       <c r="O64" s="1" t="b">
-        <f>IF(N64&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P64" s="1" t="b">
@@ -10649,15 +10672,15 @@
         <v>125</v>
       </c>
       <c r="M65" s="2" t="str">
-        <f>_xlfn.CONCAT(I65,L65,J65)</f>
+        <f t="shared" si="3"/>
         <v>QVQLVQSGAEVKKPGSSVKVSCKASGGTFSSYSFIWVRQAPGQGLEWMGGIIPIFGTANYAQKFQGRVTITADESTSTAYMELSSLRSEDTAVYYCARSSYSGVYYSWYFDVWGAGTTVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQGISNYLAWYQQKPGKAPKLLIYAASTLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQQSYSTPRTFGQGTKVEIK</v>
       </c>
       <c r="N65" s="4">
-        <f>LEN(M65)</f>
+        <f t="shared" si="4"/>
         <v>246</v>
       </c>
       <c r="O65" s="1" t="b">
-        <f>IF(N65&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P65" s="1" t="b">
@@ -10708,15 +10731,15 @@
         <v>125</v>
       </c>
       <c r="M66" s="2" t="str">
-        <f>_xlfn.CONCAT(I66,L66,J66)</f>
+        <f t="shared" ref="M66:M97" si="6">_xlfn.CONCAT(I66,L66,J66)</f>
         <v>EVQLQESGPGLVKPSQTLSLTCTVSGGSISSYAAWSWIRQPPGKGLEWIGYIYSSSGSTNYNPSLKSRVTISVDTSKNQFSLKLSSVTAADTAVYYCARGDYSYSYYGLDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQGIRNDLGWYQQKPGKAPKLLIYAASNLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQQSYSTPRYTFGQGTKVEIK</v>
       </c>
       <c r="N66" s="4">
-        <f>LEN(M66)</f>
+        <f t="shared" ref="N66:N97" si="7">LEN(M66)</f>
         <v>246</v>
       </c>
       <c r="O66" s="1" t="b">
-        <f>IF(N66&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" ref="O66:O97" si="8">IF(N66&lt;=250,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="P66" s="1" t="b">
@@ -10767,15 +10790,15 @@
         <v>125</v>
       </c>
       <c r="M67" s="2" t="str">
-        <f>_xlfn.CONCAT(I67,L67,J67)</f>
+        <f t="shared" si="6"/>
         <v>EVQLQQSGPELVKPGASVKMSCKASGYTFTSYNIHWVKQTPVHGLEWIGAIVSGGDTNYNENFKDKATLTVDKSSSTAYMQLTSEDSAVYYCARGGFYGDYWGQGTSVTVSSGGGSGGGSGGGSGGGSDIVLTQSPATLSVTPGDSVSLSCRASQSVTNNIHWYQQKSHESPRLLIKYASQSISGIPSRFSGSGSGTDFTLSINSVETEDFGMYFCQQSNSWPYTFGGGTKLEIK</v>
       </c>
       <c r="N67" s="4">
-        <f>LEN(M67)</f>
+        <f t="shared" si="7"/>
         <v>235</v>
       </c>
       <c r="O67" s="1" t="b">
-        <f>IF(N67&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P67" s="1" t="b">
@@ -10826,15 +10849,15 @@
         <v>125</v>
       </c>
       <c r="M68" s="2" t="str">
-        <f>_xlfn.CONCAT(I68,L68,J68)</f>
+        <f t="shared" si="6"/>
         <v>QVQLQESGPGLVKPSQTLSLTCTVSGGSISSGDYYWIRQHPGKGLEWIGYIYYSGSTYYNPSLKSRVTISVDTSKNQFSLKLSSVTAADTAVYYCARQLWLRGRFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQGISSWLAWYQQKPGKAPKLLIYAASTLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQQSYSTPYTFGQGTKVEIK</v>
       </c>
       <c r="N68" s="4">
-        <f>LEN(M68)</f>
+        <f t="shared" si="7"/>
         <v>241</v>
       </c>
       <c r="O68" s="1" t="b">
-        <f>IF(N68&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P68" s="1" t="b">
@@ -10885,15 +10908,15 @@
         <v>125</v>
       </c>
       <c r="M69" s="2" t="str">
-        <f>_xlfn.CONCAT(I69,L69,J69)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFTVSSNYMSWVRQAPGKGLEWVSVIYSGGSTYYADSVKGRFTISRDNSKNTLYLQMNSLRAEDTAVYYCAREAGVWVFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N69" s="4">
-        <f>LEN(M69)</f>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="O69" s="1" t="b">
-        <f>IF(N69&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P69" s="1" t="b">
@@ -10944,15 +10967,15 @@
         <v>125</v>
       </c>
       <c r="M70" s="2" t="str">
-        <f>_xlfn.CONCAT(I70,L70,J70)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNLYSSSIHWVRQAPGKGLEWVASISSYYGSTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARSRQFWLWFGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N70" s="4">
-        <f>LEN(M70)</f>
+        <f t="shared" si="7"/>
         <v>239</v>
       </c>
       <c r="O70" s="1" t="b">
-        <f>IF(N70&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P70" s="1" t="b">
@@ -10998,15 +11021,15 @@
         <v>125</v>
       </c>
       <c r="M71" s="2" t="str">
-        <f>_xlfn.CONCAT(I71,L71,J71)</f>
+        <f t="shared" si="6"/>
         <v>VQLVQSGAEVKKPGASVKVSCKASGYTFTTYTISWVRQAPGQGLEWMGWINNSGGTNYAQKFQGRVTMTRDTSTSTVSAYMELRSEDTAVYYCATFVYGYSAYQPLTDDYGQMDVWGQGTTVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSISSYLNWFQQKPGKAPKLLIYAASSLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQQSLLYPLTFGGGTKVEIK</v>
       </c>
       <c r="N71" s="4">
-        <f>LEN(M71)</f>
+        <f t="shared" si="7"/>
         <v>249</v>
       </c>
       <c r="O71" s="1" t="b">
-        <f>IF(N71&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P71" s="1" t="b">
@@ -11057,15 +11080,15 @@
         <v>125</v>
       </c>
       <c r="M72" s="2" t="str">
-        <f>_xlfn.CONCAT(I72,L72,J72)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNISSSSIHWVRQAPGKGLEWVASIYSSSGSTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARHRWWAHPYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQSYYITPYTFGQGTKVEIK</v>
       </c>
       <c r="N72" s="4">
-        <f>LEN(M72)</f>
+        <f t="shared" si="7"/>
         <v>241</v>
       </c>
       <c r="O72" s="1" t="b">
-        <f>IF(N72&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P72" s="1" t="b">
@@ -11116,15 +11139,15 @@
         <v>125</v>
       </c>
       <c r="M73" s="2" t="str">
-        <f>_xlfn.CONCAT(I73,L73,J73)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGVVQPGRSLRLSCAASGFTFSSYAMHWVRQAPGKGLEWVAVIWYDGSNKYYADSVKGRFTISRDNSKNTLFLQMNSLRPEDTAVYYCARDTPMYYDVWGQGTTVTVSSGGGSGGGSGGGSGGGSDIQLTQSPSSLSASVGDRVTITCRTSQDIDNYLNWYQQKPGKAPKLLIYYTSSLHSGVPSRFSGSGSGTDFTFTISSLQPEDIATYYCQQYDNLPITFGQGTKLEIK</v>
       </c>
       <c r="N73" s="4">
-        <f>LEN(M73)</f>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="O73" s="1" t="b">
-        <f>IF(N73&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P73" s="1" t="b">
@@ -11175,15 +11198,15 @@
         <v>125</v>
       </c>
       <c r="M74" s="2" t="str">
-        <f>_xlfn.CONCAT(I74,L74,J74)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFTFSNYAMSWVRQAPGKGLEWVSAISGSGGSTYYADSVKGRFTISRDNSKNTLYLQMNSLRAEDTAVYYCARLSPYNGSMDYWGQGTLVTVSSGGGSGGGSGGGSGGGSVTQPASVSGSPGQSITISCTGTSSDIGAYNYVSWYQQHPGKAPKLMIYEVSKRPSGVSNRFSGSKSGNTASLTISGLQTEDEADYYCSSYTRSGSVVFGGGTKLTVL</v>
       </c>
       <c r="N74" s="4">
-        <f>LEN(M74)</f>
+        <f t="shared" si="7"/>
         <v>242</v>
       </c>
       <c r="O74" s="1" t="b">
-        <f>IF(N74&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P74" s="1" t="b">
@@ -11234,15 +11257,15 @@
         <v>125</v>
       </c>
       <c r="M75" s="2" t="str">
-        <f>_xlfn.CONCAT(I75,L75,J75)</f>
+        <f t="shared" si="6"/>
         <v>QVQLVQSGAEVKKPGSSVKVSCKASGGTFSSYTISWVRQAPGQGLEWMGGIIPILGIANYAQKFQGRVTITADKSTSTAYMELSSLRSEDTAVYYCARGDSSYVDSWDYWGQGTLVTVSGGGSGGGSGGGSGGGSEIVLTQSPGTLSLSPGERATLSCRASQSVSSSYLAWYQQKPGQAPRLLIYGASSRATGIPDRFSGSGSGTDFTLTISRLEPEDFAVYYCQQYGSSPWTFGQGTKVEIK</v>
       </c>
       <c r="N75" s="4">
-        <f>LEN(M75)</f>
+        <f t="shared" si="7"/>
         <v>243</v>
       </c>
       <c r="O75" s="1" t="b">
-        <f>IF(N75&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P75" s="1" t="b">
@@ -11293,15 +11316,15 @@
         <v>125</v>
       </c>
       <c r="M76" s="2" t="str">
-        <f>_xlfn.CONCAT(I76,L76,J76)</f>
+        <f t="shared" si="6"/>
         <v>QVQLVESGGGVVQPGRSLRLSCAASGFTFSNYGMHWVRQAPGKGLEWVAVISDGSNKYYADSVKGRFTISRDNSKNTLYLQMRAEDTAVYYCARGSHSSRDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSISSYLNWYQQKPGKAPKLLIYAASSLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQQSYSTPPYTFGQGTKVEIK</v>
       </c>
       <c r="N76" s="4">
-        <f>LEN(M76)</f>
+        <f t="shared" si="7"/>
         <v>237</v>
       </c>
       <c r="O76" s="1" t="b">
-        <f>IF(N76&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P76" s="1" t="b">
@@ -11352,15 +11375,15 @@
         <v>125</v>
       </c>
       <c r="M77" s="2" t="str">
-        <f>_xlfn.CONCAT(I77,L77,J77)</f>
+        <f t="shared" si="6"/>
         <v>VQLVQSGAEVKRPGSSVKVSCKTSGGTIFSTYVFWVRQAPGQGLEWMGGFPPKAGYIYAQKFQGRVTFTADESSSTTVYMEDLRSEDTAVYFCARFPYFVYDVWGQGTTVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSIGGYLAWYQQKPGKVPKLLIYAASSLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQQSYSTPRTFGQGTKVEIK</v>
       </c>
       <c r="N77" s="4">
-        <f>LEN(M77)</f>
+        <f t="shared" si="7"/>
         <v>237</v>
       </c>
       <c r="O77" s="1" t="b">
-        <f>IF(N77&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P77" s="1" t="b">
@@ -11411,15 +11434,15 @@
         <v>126</v>
       </c>
       <c r="M78" s="2" t="str">
-        <f>_xlfn.CONCAT(I78,L78,J78)</f>
+        <f t="shared" si="6"/>
         <v>VQLQESGPGLVKPSQSLSLTCTVTGFSIDYNIYWGWIRQPPGKGLEWIGYIYSGSDTYNPSLKSRVTISVDTSKNQFSLKVNSVTAADTAVYYCARVVDLWYDDGKYASCVKGAIDYWGQGTLVTVSSGGGSGGGSGGGSSVLTQPPSVSGAPGQRVTISCTGSSGAGYDVHWYQQLPGTAPKLLIYGNSNRPSGVPDRFSGSKSGTSASLAITGLQAEDEADYYCQSYDSSLSGWVFGGGTKLTVL</v>
       </c>
       <c r="N78" s="4">
-        <f>LEN(M78)</f>
+        <f t="shared" si="7"/>
         <v>247</v>
       </c>
       <c r="O78" s="1" t="b">
-        <f>IF(N78&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P78" s="1" t="b">
@@ -11470,15 +11493,15 @@
         <v>125</v>
       </c>
       <c r="M79" s="2" t="str">
-        <f>_xlfn.CONCAT(I79,L79,J79)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVVDFSLHWVRQAPGKGLEWVASIYPYDGSAYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARWGYWPGEGWLGKYWGQGTLVTVSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEI</v>
       </c>
       <c r="N79" s="4">
-        <f>LEN(M79)</f>
+        <f t="shared" si="7"/>
         <v>243</v>
       </c>
       <c r="O79" s="1" t="b">
-        <f>IF(N79&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P79" s="1" t="b">
@@ -11529,15 +11552,15 @@
         <v>125</v>
       </c>
       <c r="M80" s="2" t="str">
-        <f>_xlfn.CONCAT(I80,L80,J80)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNISSSSIHWVRQAPGKGLEWVASISSSYGSTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARWEGYRGDLWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYYEWLRTFGQGTKVEIK</v>
       </c>
       <c r="N80" s="4">
-        <f>LEN(M80)</f>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="O80" s="1" t="b">
-        <f>IF(N80&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P80" s="1" t="b">
@@ -11594,15 +11617,15 @@
         <v>125</v>
       </c>
       <c r="M81" s="2" t="str">
-        <f>_xlfn.CONCAT(I81,L81,J81)</f>
+        <f t="shared" si="6"/>
         <v>QVQLQESGPGLVKPSQTLSLTCTVSGGSVSSGSYYWSWIRQPPGKGLEWIGYIYYSGSTNYNPSLKSRVTISVDTSKNQFSLKLSSVTAADTAVYYCARVDSFYYGMDVWGQGTTVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASSGSSYDNGWYQQKPGKAPKLLIYAASSLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYLQDSNYTPRTFGQGTKVEIK</v>
       </c>
       <c r="N81" s="4">
-        <f>LEN(M81)</f>
+        <f t="shared" si="7"/>
         <v>243</v>
       </c>
       <c r="O81" s="1" t="b">
-        <f>IF(N81&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P81" s="1" t="b">
@@ -11659,15 +11682,15 @@
         <v>125</v>
       </c>
       <c r="M82" s="2" t="str">
-        <f>_xlfn.CONCAT(I82,L82,J82)</f>
+        <f t="shared" si="6"/>
         <v>QVQLVQSGAEVKKPGSSVKVSCKASGGTFSSYTISWVRQAPGQGLEWMGRIIPIFGTANYAQKFQGRVTITADKSTSTAYMELSSLRSEDTAVYYCARYYDSYFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQGISSWLAWYQQKPGKAPKLLIYAASSLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQCGNSFPWTFGGGTKLEIK</v>
       </c>
       <c r="N82" s="4">
-        <f>LEN(M82)</f>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="O82" s="1" t="b">
-        <f>IF(N82&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P82" s="1" t="b">
@@ -11718,15 +11741,15 @@
         <v>125</v>
       </c>
       <c r="M83" s="2" t="str">
-        <f>_xlfn.CONCAT(I83,L83,J83)</f>
+        <f t="shared" si="6"/>
         <v>DVQLQESGPGLVKPSQTLSLTCTVSGYSITSDYYWNWIRQFPGNKLEWMGYISYDGSSNYNPSLKNRISITRDNSKNQFFLQLNSVTTEDTATYYCARSCSRRGYAMDYWGQGTSVTVSSGGGSGGGSGGGSGGGSQIVLTQSPAIMSASLGEKVTLTCSASSSVSYMHWYQQKPGTSPKLLIYSCNLLSGVPDRFSGSGSGTDFTLSISNVETEDAATYYCYQYRIRFGGGTKLTVLQ</v>
       </c>
       <c r="N83" s="4">
-        <f>LEN(M83)</f>
+        <f t="shared" si="7"/>
         <v>239</v>
       </c>
       <c r="O83" s="1" t="b">
-        <f>IF(N83&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P83" s="1" t="b">
@@ -11777,15 +11800,15 @@
         <v>125</v>
       </c>
       <c r="M84" s="2" t="str">
-        <f>_xlfn.CONCAT(I84,L84,J84)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFTFSSYAMSWVRQAPGKGLEWVSSISRSGGSTYYADSVKGRFTISRDNAKNSLYLQMNSLRAEDTAVYYCARSCSSRGYFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIVMTQSPDSLAVSLGERATINCRASQSVSSYLAWYQQKPGQSPKLLIYSCNLQSGVPDRFSGSGSGTDFTLTISSLQPEDFATYYCQPYIRFGGGGTKLEIK</v>
       </c>
       <c r="N84" s="4">
-        <f>LEN(M84)</f>
+        <f t="shared" si="7"/>
         <v>238</v>
       </c>
       <c r="O84" s="1" t="b">
-        <f>IF(N84&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P84" s="1" t="b">
@@ -11836,15 +11859,15 @@
         <v>125</v>
       </c>
       <c r="M85" s="2" t="str">
-        <f>_xlfn.CONCAT(I85,L85,J85)</f>
+        <f t="shared" si="6"/>
         <v>QVQLQESGPGLVKPSQTLSLTCTVSGFSFSSYAMSWVRQAPGKGLEWVSSISRSGGSTYYADSVKGRFTISRDNAKNSLYLQMNSLRAEDTAVYYCARSCSSRGYLFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIVMTQSPDSLAVSLGERATINCRASQSVSSYLAWYQQKPGQSPKLLIYSCNLQSGVPDRFSGSGSGTDFTLTISSLQPEDFATYYCQPYIRFGGGGTKLEIK</v>
       </c>
       <c r="N85" s="4">
-        <f>LEN(M85)</f>
+        <f t="shared" si="7"/>
         <v>239</v>
       </c>
       <c r="O85" s="1" t="b">
-        <f>IF(N85&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P85" s="1" t="b">
@@ -11898,15 +11921,15 @@
         <v>125</v>
       </c>
       <c r="M86" s="2" t="str">
-        <f>_xlfn.CONCAT(I86,L86,J86)</f>
+        <f t="shared" si="6"/>
         <v>SIKLTESGPTSVAPGSTLNLTCTVTGDNITSSGWYWWVKQAPDNKLTWIGGIDKNGNTWLNVAYIDRATLTRDPAANTVYLSIRNVTSSDTATYYCAKSSDDNGSYLDVWGQGLKVTVSGGGGSGGGSGGGSGGGSQVKLTQSPKEVTAKIGDTVTLTCTASQPVSTVSWYMQKPGQPPQLLISNNKLVEGVPERFSASGSGTEFTLTIKDVQKEDEAIYYCEVNGQVFGQGTKLTVLE</v>
       </c>
       <c r="N86" s="4">
-        <f>LEN(M86)</f>
+        <f t="shared" si="7"/>
         <v>239</v>
       </c>
       <c r="O86" s="1" t="b">
-        <f>IF(N86&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P86" s="1" t="b">
@@ -11957,15 +11980,15 @@
         <v>125</v>
       </c>
       <c r="M87" s="2" t="str">
-        <f>_xlfn.CONCAT(I87,L87,J87)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVSYSSIHWVRQAPGKGLEWVASIYSYSGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARGWYSYFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N87" s="4">
-        <f>LEN(M87)</f>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="O87" s="1" t="b">
-        <f>IF(N87&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P87" s="1" t="b">
@@ -12011,15 +12034,15 @@
         <v>125</v>
       </c>
       <c r="M88" s="2" t="str">
-        <f>_xlfn.CONCAT(I88,L88,J88)</f>
+        <f t="shared" si="6"/>
         <v>QVQLVQSGAEVKKPGSSVKVSCKASGGTFSSYAISWVRQAPGQGLEWMGGIIIFGTANYAQKFQGRVTITADKSTSTAYMELRSEDTAVYYCAREGTTGWDYWGQGTLVTVSSGGGSGGGSGGGSGGGSEIVLTQSPGTLSLSPGERATLSCRASQSVSSSYLAWYQQKPGQAPRLLIYGASSRATGIPDRFSGSGSGTDFTLTISRLEPEDFAVYYCQQYGSSPRTFGQGTKVEIK</v>
       </c>
       <c r="N88" s="4">
-        <f>LEN(M88)</f>
+        <f t="shared" si="7"/>
         <v>237</v>
       </c>
       <c r="O88" s="1" t="b">
-        <f>IF(N88&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P88" s="1" t="b">
@@ -12070,15 +12093,15 @@
         <v>125</v>
       </c>
       <c r="M89" s="2" t="str">
-        <f>_xlfn.CONCAT(I89,L89,J89)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVSYYSIHWVRQAPGKGLEWVASIYSYSGYTSYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARYYVYYGAMDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N89" s="4">
-        <f>LEN(M89)</f>
+        <f t="shared" si="7"/>
         <v>242</v>
       </c>
       <c r="O89" s="1" t="b">
-        <f>IF(N89&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P89" s="1" t="b">
@@ -12126,15 +12149,15 @@
         <v>125</v>
       </c>
       <c r="M90" s="2" t="str">
-        <f>_xlfn.CONCAT(I90,L90,J90)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVSYSSIHWVRQAPGKGLEWVASIYSYSGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARGWVRGSSYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N90" s="4">
-        <f>LEN(M90)</f>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="O90" s="1" t="b">
-        <f>IF(N90&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P90" s="1" t="b">
@@ -12185,15 +12208,15 @@
         <v>125</v>
       </c>
       <c r="M91" s="2" t="str">
-        <f>_xlfn.CONCAT(I91,L91,J91)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVSYSSIHWVRQAPGKGLEWVASIYSYSGYTNYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARYYGGYGGYFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N91" s="4">
-        <f>LEN(M91)</f>
+        <f t="shared" si="7"/>
         <v>243</v>
       </c>
       <c r="O91" s="1" t="b">
-        <f>IF(N91&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P91" s="1" t="b">
@@ -12239,15 +12262,15 @@
         <v>125</v>
       </c>
       <c r="M92" s="2" t="str">
-        <f>_xlfn.CONCAT(I92,L92,J92)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVSYYSIHWVRQAPGKGLEWVASIYPYSGYTNYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARYYGYWYFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N92" s="4">
-        <f>LEN(M92)</f>
+        <f t="shared" si="7"/>
         <v>241</v>
       </c>
       <c r="O92" s="1" t="b">
-        <f>IF(N92&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P92" s="1" t="b">
@@ -12293,15 +12316,15 @@
         <v>125</v>
       </c>
       <c r="M93" s="2" t="str">
-        <f>_xlfn.CONCAT(I93,L93,J93)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVSYSSIHWVRQAPGKGLEWVASIYSYSGYTSYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARYYGGYGGWYFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N93" s="4">
-        <f>LEN(M93)</f>
+        <f t="shared" si="7"/>
         <v>244</v>
       </c>
       <c r="O93" s="1" t="b">
-        <f>IF(N93&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P93" s="1" t="b">
@@ -12347,15 +12370,15 @@
         <v>125</v>
       </c>
       <c r="M94" s="2" t="str">
-        <f>_xlfn.CONCAT(I94,L94,J94)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVSYYSIHWVRQAPGKGLEWVASISSYYGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARYYGYWYFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N94" s="4">
-        <f>LEN(M94)</f>
+        <f t="shared" si="7"/>
         <v>241</v>
       </c>
       <c r="O94" s="1" t="b">
-        <f>IF(N94&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P94" s="1" t="b">
@@ -12401,15 +12424,15 @@
         <v>125</v>
       </c>
       <c r="M95" s="2" t="str">
-        <f>_xlfn.CONCAT(I95,L95,J95)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVSYYSIHWVRQAPGKGLEWVASISSYYGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARYYGTYYGHSYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N95" s="4">
-        <f>LEN(M95)</f>
+        <f t="shared" si="7"/>
         <v>242</v>
       </c>
       <c r="O95" s="1" t="b">
-        <f>IF(N95&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P95" s="1" t="b">
@@ -12455,15 +12478,15 @@
         <v>125</v>
       </c>
       <c r="M96" s="2" t="str">
-        <f>_xlfn.CONCAT(I96,L96,J96)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVSYSSIHWVRQAPGKGLEWVASIYSYSGYTNYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARYWYFGYFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N96" s="4">
-        <f>LEN(M96)</f>
+        <f t="shared" si="7"/>
         <v>241</v>
       </c>
       <c r="O96" s="1" t="b">
-        <f>IF(N96&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P96" s="1" t="b">
@@ -12509,15 +12532,15 @@
         <v>125</v>
       </c>
       <c r="M97" s="2" t="str">
-        <f>_xlfn.CONCAT(I97,L97,J97)</f>
+        <f t="shared" si="6"/>
         <v>EVQLVESGGGLVKPGGSLRLSCAASGFTFRNYAMSWVRQAPGKGLEWVSSISSKSKSTSYADSVKGRFTISRDNAKNSLYLQMNSLRAEDTAVYYCARESGSFSYEGVWGQGTLVTVSSGGGSGGGSGGGSGGGSSVLTQPPSVSGAPGQRVTISCTGSSSNIGAGYDVHWYQQLPGTAPKLLIYDNNKRPSGVPDRFSGSKSGTSASLAITGLQAEDEADYYCQSYDSSLSGLVFGGGTKLTVL</v>
       </c>
       <c r="N97" s="4">
-        <f>LEN(M97)</f>
+        <f t="shared" si="7"/>
         <v>245</v>
       </c>
       <c r="O97" s="1" t="b">
-        <f>IF(N97&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P97" s="1" t="b">
@@ -12568,15 +12591,15 @@
         <v>125</v>
       </c>
       <c r="M98" s="2" t="str">
-        <f>_xlfn.CONCAT(I98,L98,J98)</f>
+        <f t="shared" ref="M98:M129" si="9">_xlfn.CONCAT(I98,L98,J98)</f>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNISSSSIHWVRQAPGKGLEWVASIYYSSGYTHYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARWGYWPGQVWLWFAYWGQGTLVTVSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQSSSSLITFGQGTKVEIK</v>
       </c>
       <c r="N98" s="4">
-        <f>LEN(M98)</f>
+        <f t="shared" ref="N98:N129" si="10">LEN(M98)</f>
         <v>245</v>
       </c>
       <c r="O98" s="1" t="b">
-        <f>IF(N98&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" ref="O98:O129" si="11">IF(N98&lt;=250,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="P98" s="1" t="b">
@@ -12627,15 +12650,15 @@
         <v>125</v>
       </c>
       <c r="M99" s="2" t="str">
-        <f>_xlfn.CONCAT(I99,L99,J99)</f>
+        <f t="shared" si="9"/>
         <v>QVQLVQSGAEVKKPGSSVKVSCKSSGGTSNNYAISWVRQAPGQGLEWMGGIIPILGIANYAQKFQGRVTITADKSTSTAYMELSSLRSEDTAVYYCAREDAVVDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSTLSASVGDRVTITCRASQGISSWLAWYQQKPGKAPKLLIYKASSLESGVPSRFSGSGSGTEFTLTISSLQPDDFATYYCQQYNSYPLTFGQGTKVQVK</v>
       </c>
       <c r="N99" s="4">
-        <f>LEN(M99)</f>
+        <f t="shared" si="10"/>
         <v>239</v>
       </c>
       <c r="O99" s="1" t="b">
-        <f>IF(N99&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P99" s="1" t="b">
@@ -12686,15 +12709,15 @@
         <v>125</v>
       </c>
       <c r="M100" s="2" t="str">
-        <f>_xlfn.CONCAT(I100,L100,J100)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNVSSSSIHWVRQAPGKGLEWVASISSYYGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARHWGYCSWFAYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N100" s="4">
-        <f>LEN(M100)</f>
+        <f t="shared" si="10"/>
         <v>242</v>
       </c>
       <c r="O100" s="1" t="b">
-        <f>IF(N100&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P100" s="1" t="b">
@@ -12740,15 +12763,15 @@
         <v>125</v>
       </c>
       <c r="M101" s="2" t="str">
-        <f>_xlfn.CONCAT(I101,L101,J101)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNISSSSIHWVRQAPGKGLEWVASIYSYSGYTSYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARGSHYFGYFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQSSSSLITFGQGTKVEIK</v>
       </c>
       <c r="N101" s="4">
-        <f>LEN(M101)</f>
+        <f t="shared" si="10"/>
         <v>242</v>
       </c>
       <c r="O101" s="1" t="b">
-        <f>IF(N101&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P101" s="1" t="b">
@@ -12794,15 +12817,15 @@
         <v>125</v>
       </c>
       <c r="M102" s="2" t="str">
-        <f>_xlfn.CONCAT(I102,L102,J102)</f>
+        <f t="shared" si="9"/>
         <v>QVQLQESGPGLVKPSQTLSLTCTVSGGSISSGDYYWIRQHPGKGLEWIGYIYYSGSTDYNPSLKSRVTISVDTSKNQFSLKVTAADTAVYYCARTWFGSDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQGISNYLAWYQQKPGKAPKLLIYAASTLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQQAHSFPYTFGGGTKLEIK</v>
       </c>
       <c r="N102" s="4">
-        <f>LEN(M102)</f>
+        <f t="shared" si="10"/>
         <v>235</v>
       </c>
       <c r="O102" s="1" t="b">
-        <f>IF(N102&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P102" s="1" t="b">
@@ -12853,15 +12876,15 @@
         <v>125</v>
       </c>
       <c r="M103" s="2" t="str">
-        <f>_xlfn.CONCAT(I103,L103,J103)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFTFSSYWMNWVRQAPGKGLEWVAFIRYDGGNKYYADSVKGRFTISRDNSKNTLYLQMNSLRAEDTAVYYCARWSYSGGSGSYYVYFDYWGQGTLVTVSGGGSGGGSGGGSGGGSSVLTQPPSVSGAPGQRVTISCTGSSSNIGAGYDVHWYQQLPGTAPKLLIYGNSNRPSGVPDRFSGSKSGTSASLAITGLQAEDEADYYCQSYDSSLSGSVFGGGTKLTVL</v>
       </c>
       <c r="N103" s="4">
-        <f>LEN(M103)</f>
+        <f t="shared" si="10"/>
         <v>250</v>
       </c>
       <c r="O103" s="1" t="b">
-        <f>IF(N103&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P103" s="1" t="b">
@@ -12912,15 +12935,15 @@
         <v>125</v>
       </c>
       <c r="M104" s="2" t="str">
-        <f>_xlfn.CONCAT(I104,L104,J104)</f>
+        <f t="shared" si="9"/>
         <v>QVQLVQSGAEVKKPGASVKVSCKASGYTFTNYYIHWVRQAPGQGLEWMGWIYPGGNTNYAQKFQGRVTMTRDTSISTAYMELSRLRSDDTAVYYCARVRTEFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIVMTQSPSSLAMSAGAETITCRSSQSVHSNGYLNWYQQKPGQPPKLLIYWASTRESGVPDRFTGSGSGTDFTLTITNVQSEDLAEYFCQQYSSYPLTFGAGTKLELR</v>
       </c>
       <c r="N104" s="4">
-        <f>LEN(M104)</f>
+        <f t="shared" si="10"/>
         <v>239</v>
       </c>
       <c r="O104" s="1" t="b">
-        <f>IF(N104&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P104" s="1" t="b">
@@ -12971,15 +12994,15 @@
         <v>125</v>
       </c>
       <c r="M105" s="2" t="str">
-        <f>_xlfn.CONCAT(I105,L105,J105)</f>
+        <f t="shared" si="9"/>
         <v>QVQLQESGPGLVKPSETLSLTCTVSGGSVSSGGYFWSWIRQPPGKGLEWIGYVSGSGSTNYNPSLKSRVTISVDTSKNQFSLKLSSVTAADTAVYYCARWDVWISDYWGQGTLVTVSSGGGSGGGSGGGSGGGSEIVLTQSPATLSLSPGERATLSCRASQSVSSYLAWYQQKPGQAPRLLIYDASNRATGIPARFSGSGSGTDFTLTISSLEPEDFAVYYCQHSWDQPPWTFGQGTKVEIK</v>
       </c>
       <c r="N105" s="4">
-        <f>LEN(M105)</f>
+        <f t="shared" si="10"/>
         <v>242</v>
       </c>
       <c r="O105" s="1" t="b">
-        <f>IF(N105&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P105" s="1" t="b">
@@ -13030,15 +13053,15 @@
         <v>125</v>
       </c>
       <c r="M106" s="2" t="str">
-        <f>_xlfn.CONCAT(I106,L106,J106)</f>
+        <f t="shared" si="9"/>
         <v>QVQLQESGPGLVKPSQTLSLTCTVTGSSITSGYWNWIRQFPGNKLEWMGYISYSGTITYNPSLKSRISITRDTSKNQFFLQLNSVTTEDTATYYCARVYDGFYDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIVMTQSPSSLSASVGDRVTITCRASQGISSWLAWYQQKPGKAPKLLIYKASSLESGVPSRFSGSGSGTEFTLTISSLQPDDFATYYCQQYNSYPLTFGGGTKVEIK</v>
       </c>
       <c r="N106" s="4">
-        <f>LEN(M106)</f>
+        <f t="shared" si="10"/>
         <v>239</v>
       </c>
       <c r="O106" s="1" t="b">
-        <f>IF(N106&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P106" s="1" t="b">
@@ -13089,15 +13112,15 @@
         <v>125</v>
       </c>
       <c r="M107" s="2" t="str">
-        <f>_xlfn.CONCAT(I107,L107,J107)</f>
+        <f t="shared" si="9"/>
         <v>QVQLVESGGGVVQPGRSLRLSCAASGFTFSNYAMHWVRQAPGKGLEWVAVISYNSGNPYADSVKGRFTISRDNSKNTLYLQMRVEDTAVYYCSRTTIGYGGDIWGNMFDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIVMTQSPATLSVSPGDRATLSCRASQSISTNLAWYQQKPGQAPRLLIYTASTLESGVPSRFSGSGSGTEFTLTISNLQSEDFATYFCQQYSAPLTFGGGTKVEIK</v>
       </c>
       <c r="N107" s="4">
-        <f>LEN(M107)</f>
+        <f t="shared" si="10"/>
         <v>243</v>
       </c>
       <c r="O107" s="1" t="b">
-        <f>IF(N107&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P107" s="1" t="b">
@@ -13148,15 +13171,15 @@
         <v>126</v>
       </c>
       <c r="M108" s="2" t="str">
-        <f>_xlfn.CONCAT(I108,L108,J108)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFASSSSNYVHWVRQAPGKGLEWVATIYPYSSSEYAASVQGRFTISRDDSKNTLYLQMNSLRGEDTAVYYCARYGYYSSRSGYGYYFNYWGQGTLVTVSSGGGSGGGSGGGSDIVMTQSPASLAVSLGQRATISCRASESVDSYGNSFLAWYQQKPGQPPKLLIYWASTRQSGVPARFSGSGSGTDFTLNIHPVEEEDAATYYCQQHNYPLTFGAGTKLEIK</v>
       </c>
       <c r="N108" s="4">
-        <f>LEN(M108)</f>
+        <f t="shared" si="10"/>
         <v>247</v>
       </c>
       <c r="O108" s="1" t="b">
-        <f>IF(N108&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P108" s="1" t="b">
@@ -13207,15 +13230,15 @@
         <v>125</v>
       </c>
       <c r="M109" s="2" t="str">
-        <f>_xlfn.CONCAT(I109,L109,J109)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVESGAEVKKPGSSVKVSCKASGGPFTSYVISWVRQAPGQGLEWMGRIIPIRGTTYAQKFQGRVTITADKSTSTAYMELRSEDTAVYYCARGSHVFGYYDYWGQGTLVTVSSGGGSGGGSGGGSGGGSEIVLTQSPGTLSLSPGERATLSCRASQSISGNYLAWYQQKPGQAPRLLIYGASIRAAGIPDRFSGSGSGTDFTLTISRLEPEDFAVYYCQQYGSSPRTFGQGTKVEIK</v>
       </c>
       <c r="N109" s="4">
-        <f>LEN(M109)</f>
+        <f t="shared" si="10"/>
         <v>239</v>
       </c>
       <c r="O109" s="1" t="b">
-        <f>IF(N109&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P109" s="1" t="b">
@@ -13266,15 +13289,15 @@
         <v>125</v>
       </c>
       <c r="M110" s="2" t="str">
-        <f>_xlfn.CONCAT(I110,L110,J110)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVETGGGLVQPGGSLKLSCRASGYTFTDYAMHWVRQAPLGLGLYTGGVNYARHFMKSRISITRDNSKNTLYLQMTKVDDTATYFCARRGLFDSDYWGQGTLVTVSSGGGSGGGSGGGSGGGSSVTQPPSVSGSTSVGDRVTTCRASQSISSNWLAWYQQFPGTAPKLLIYENSSRPSGVPDRFSGSGSGTDFTLKISRVEAEDVGVYYCLQALSPRFTFGSGTKLEIK</v>
       </c>
       <c r="N110" s="4">
-        <f>LEN(M110)</f>
+        <f t="shared" si="10"/>
         <v>231</v>
       </c>
       <c r="O110" s="1" t="b">
-        <f>IF(N110&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P110" s="1" t="b">
@@ -13325,15 +13348,15 @@
         <v>125</v>
       </c>
       <c r="M111" s="2" t="str">
-        <f>_xlfn.CONCAT(I111,L111,J111)</f>
+        <f t="shared" si="9"/>
         <v>QVQLVQSGAEVKKPGSSVKVSCKASGGTFSNYGISWVRQAPGQGLEWMGGIIPILGIANYAQKFQGRVTITADKSTSTAYMELRSLRSDDTAVYYCAREGHAYFHNGLDYWGQGTLVTVSSGGGSGGGSGGGSGGGSEIVLTQSPGTLSLSPGERATLSCRASQSVSSSYFAWYQQKPGQAPRLLIYGASSRATGIPDRFSGSGSGTDFTLTISRLEPEDFAVYYCQQYGSSPPATFGQGTKVEIK</v>
       </c>
       <c r="N111" s="4">
-        <f>LEN(M111)</f>
+        <f t="shared" si="10"/>
         <v>246</v>
       </c>
       <c r="O111" s="1" t="b">
-        <f>IF(N111&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P111" s="1" t="b">
@@ -13384,15 +13407,15 @@
         <v>125</v>
       </c>
       <c r="M112" s="2" t="str">
-        <f>_xlfn.CONCAT(I112,L112,J112)</f>
+        <f t="shared" si="9"/>
         <v>QVQLVESGGGVVQPGRSLRLSCAASGFTFSSFGMHWVRQAPGKGLEWVAIIWDGSNKYYADSVKGRFTISRDNSKNTLYLQMRAEDTAVYYCALDGGSFDDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSTLSTSVGDRVTITCRASQSISSWLAWYQQKPGKAPKLLIYKASTLESGVPSRFSGSGSGTEFTLTISSLQPDDFATYYCQHFYGTPITFGPGTKVD</v>
       </c>
       <c r="N112" s="4">
-        <f>LEN(M112)</f>
+        <f t="shared" si="10"/>
         <v>234</v>
       </c>
       <c r="O112" s="1" t="b">
-        <f>IF(N112&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P112" s="1" t="b">
@@ -13443,15 +13466,15 @@
         <v>125</v>
       </c>
       <c r="M113" s="2" t="str">
-        <f>_xlfn.CONCAT(I113,L113,J113)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVESGGGLVKPGGSLKVSCAASGFTFSDYSMNWVRQAPGKGLEWVSSITSGYTSIYYADSVKGRFTISRDNAKNSLYLQMNSLRAGDTAVYYCARVSDNFDYWGQGTAVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCQASQDIRFYLNWYQQKPGKAPKLLISAASTLQSGVPSRFSGSGSGTDFTLTITSLQPEDFATYYCAGYVPSYTFGPGTKVDIK</v>
       </c>
       <c r="N113" s="4">
-        <f>LEN(M113)</f>
+        <f t="shared" si="10"/>
         <v>238</v>
       </c>
       <c r="O113" s="1" t="b">
-        <f>IF(N113&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P113" s="1" t="b">
@@ -13502,15 +13525,15 @@
         <v>125</v>
       </c>
       <c r="M114" s="2" t="str">
-        <f>_xlfn.CONCAT(I114,L114,J114)</f>
+        <f t="shared" si="9"/>
         <v>EVQLQQSGAELVKPGASVKLSCKASGYTFLDYYMYWVKQRPEQGLEWIGRIDPANGNTIYAPKFQDKATLTLTTDTTSSNTAYMQLSSLTSEDSAVYYCAREGNYGYRDLAWFAYWGQGTLVTVSSGGGSGGGSGGGSGGGSAIRMTQSPSSLSASVGDTVTITCRASQSISSYLNWYQQKPGKAPKLLIYTASNLESGVPSRFSGSGSGTDYTLTISSLQPEDIATYYCQQYDNPPLTFGGGTKVEIK</v>
       </c>
       <c r="N114" s="4">
-        <f>LEN(M114)</f>
+        <f t="shared" si="10"/>
         <v>249</v>
       </c>
       <c r="O114" s="1" t="b">
-        <f>IF(N114&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P114" s="1" t="b">
@@ -13561,15 +13584,15 @@
         <v>125</v>
       </c>
       <c r="M115" s="2" t="str">
-        <f>_xlfn.CONCAT(I115,L115,J115)</f>
+        <f t="shared" si="9"/>
         <v>QVQLQESGPGLVKPSETLSLTCTVSGGSVSSGGYFWSWIRQRPGKGLEWIGHIYYSGTTNYNPSLRSRVTISRDTSKSQFSLKMDSLTSEDTALYYCARQLGLRFDIWGQGTMVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSISSYLNWYQQKPGKAPKLLIYAASSLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQQSYTTPPTFGQGTKVEIK</v>
       </c>
       <c r="N115" s="4">
-        <f>LEN(M115)</f>
+        <f t="shared" si="10"/>
         <v>241</v>
       </c>
       <c r="O115" s="1" t="b">
-        <f>IF(N115&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P115" s="1" t="b">
@@ -13620,15 +13643,15 @@
         <v>125</v>
       </c>
       <c r="M116" s="2" t="str">
-        <f>_xlfn.CONCAT(I116,L116,J116)</f>
+        <f t="shared" si="9"/>
         <v>QVQLVESGGGLVQPGGSLRLSCAASGFNLYSSSIHWVRQAPGKGLEWVARIYPSGATYYADSVKGRFTISADTSKNTAYLQMRAEDTAVYYCARSYYGDDYWGQGTLVTVSSGGGSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASFLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYSYYPFTFGQGTKVEIK</v>
       </c>
       <c r="N116" s="4">
-        <f>LEN(M116)</f>
+        <f t="shared" si="10"/>
         <v>235</v>
       </c>
       <c r="O116" s="1" t="b">
-        <f>IF(N116&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P116" s="1" t="b">
@@ -13682,15 +13705,15 @@
         <v>125</v>
       </c>
       <c r="M117" s="2" t="str">
-        <f>_xlfn.CONCAT(I117,L117,J117)</f>
+        <f t="shared" si="9"/>
         <v>EVQLLESGGGLVQPGGSLRLSCAASGFTFSSYAMSWVRQAPGKGLEWVSYISSSSSTIYYADSVKGRFTISRDNAKNSLYLQMNSLRAEDTAVYYCAKYSSYDYDYWGRGTMVTVSSGGGSGGGSGGGSGGGSDIQLTQSPSSLSASVGDRVTITCRASQGISSYLNWYQQKPGKAPKLLIYDASSLQSGVPSRFSGSGSGTDFTLTISSLQPEDFATYYCQQFYEWLRTFGQGTRLEIK</v>
       </c>
       <c r="N117" s="4">
-        <f>LEN(M117)</f>
+        <f t="shared" si="10"/>
         <v>240</v>
       </c>
       <c r="O117" s="1" t="b">
-        <f>IF(N117&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P117" s="1" t="b">
@@ -13744,15 +13767,15 @@
         <v>126</v>
       </c>
       <c r="M118" s="2" t="str">
-        <f>_xlfn.CONCAT(I118,L118,J118)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFATVSSNYMSWVRQAPGKGLEWVSVIYSCGSTYYADSVKGRFTISRDNSKNTLYLQMNSLRAEDTAVYYCARYYYDSSRSGYYYYFDYWGQGTLVTVSSGGGSGGGSGGGSDIVLTQSPASLAVSLGQRATISCKASQSVDYDGDSYMHWYQQKPGQPPKLLIYRASNLESGIPARFSGSGSRTDFTLTINPVEADDVATYYCQQSNYPLTFGSGTKVEIK</v>
       </c>
       <c r="N118" s="4">
-        <f>LEN(M118)</f>
+        <f t="shared" si="10"/>
         <v>247</v>
       </c>
       <c r="O118" s="1" t="b">
-        <f>IF(N118&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P118" s="1" t="b">
@@ -13806,15 +13829,15 @@
         <v>126</v>
       </c>
       <c r="M119" s="2" t="str">
-        <f>_xlfn.CONCAT(I119,L119,J119)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNISDSSIHWVRQAPGKGLEWVASISSYSGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARGGRDLFGLDALDYWGQGTLVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N119" s="4">
-        <f>LEN(M119)</f>
+        <f t="shared" si="10"/>
         <v>241</v>
       </c>
       <c r="O119" s="1" t="b">
-        <f>IF(N119&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P119" s="1" t="b">
@@ -13868,15 +13891,15 @@
         <v>126</v>
       </c>
       <c r="M120" s="2" t="str">
-        <f>_xlfn.CONCAT(I120,L120,J120)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNISSSSIHWVRQAPGKGLEWVASIYSYSGLTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARGGYYLDGLYALDYWGQGTLVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N120" s="4">
-        <f>LEN(M120)</f>
+        <f t="shared" si="10"/>
         <v>241</v>
       </c>
       <c r="O120" s="1" t="b">
-        <f>IF(N120&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P120" s="1" t="b">
@@ -13930,15 +13953,15 @@
         <v>126</v>
       </c>
       <c r="M121" s="2" t="str">
-        <f>_xlfn.CONCAT(I121,L121,J121)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNISSSSIHWVRQAPGKGLEWVASIYSYSGATYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARGGNHLDGLYALDYWGQGTLVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N121" s="4">
-        <f>LEN(M121)</f>
+        <f t="shared" si="10"/>
         <v>241</v>
       </c>
       <c r="O121" s="1" t="b">
-        <f>IF(N121&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P121" s="1" t="b">
@@ -13992,15 +14015,15 @@
         <v>126</v>
       </c>
       <c r="M122" s="2" t="str">
-        <f>_xlfn.CONCAT(I122,L122,J122)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNISSSSIHWVRQAPGKGLEWVASIYSYSGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARGGRYLDGLFALDYWGQGTLVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N122" s="4">
-        <f>LEN(M122)</f>
+        <f t="shared" si="10"/>
         <v>241</v>
       </c>
       <c r="O122" s="1" t="b">
-        <f>IF(N122&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P122" s="1" t="b">
@@ -14054,15 +14077,15 @@
         <v>126</v>
       </c>
       <c r="M123" s="2" t="str">
-        <f>_xlfn.CONCAT(I123,L123,J123)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNISSSSIHWVRQAPGKGLEWVASISSYSGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARGGSLLRGLSALDYWGQGTLVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N123" s="4">
-        <f>LEN(M123)</f>
+        <f t="shared" si="10"/>
         <v>241</v>
       </c>
       <c r="O123" s="1" t="b">
-        <f>IF(N123&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P123" s="1" t="b">
@@ -14116,15 +14139,15 @@
         <v>126</v>
       </c>
       <c r="M124" s="2" t="str">
-        <f>_xlfn.CONCAT(I124,L124,J124)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNISDSSIHWVRQAPGKGLEWVASISSYSGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARGGRYLDGLYALDYWGQGTLVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N124" s="4">
-        <f>LEN(M124)</f>
+        <f t="shared" si="10"/>
         <v>241</v>
       </c>
       <c r="O124" s="1" t="b">
-        <f>IF(N124&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P124" s="1" t="b">
@@ -14178,15 +14201,15 @@
         <v>126</v>
       </c>
       <c r="M125" s="2" t="str">
-        <f>_xlfn.CONCAT(I125,L125,J125)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNISSSSIHWVRQAPGKGLEWVASISSYSGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARGGSYLDGLSALDYWGQGTLVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N125" s="4">
-        <f>LEN(M125)</f>
+        <f t="shared" si="10"/>
         <v>241</v>
       </c>
       <c r="O125" s="1" t="b">
-        <f>IF(N125&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P125" s="1" t="b">
@@ -14240,15 +14263,15 @@
         <v>126</v>
       </c>
       <c r="M126" s="2" t="str">
-        <f>_xlfn.CONCAT(I126,L126,J126)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNISDSSIHWVRQAPGKGLEWVASIYNYSGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARGGYYLDGLDALDYWGQGTLVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N126" s="4">
-        <f>LEN(M126)</f>
+        <f t="shared" si="10"/>
         <v>241</v>
       </c>
       <c r="O126" s="1" t="b">
-        <f>IF(N126&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P126" s="1" t="b">
@@ -14302,15 +14325,15 @@
         <v>126</v>
       </c>
       <c r="M127" s="2" t="str">
-        <f>_xlfn.CONCAT(I127,L127,J127)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNISDYSIHWVRQAPGKGLEWVASIYNRSGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARGGYYLDGLYALDYWGQGTLVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N127" s="4">
-        <f>LEN(M127)</f>
+        <f t="shared" si="10"/>
         <v>241</v>
       </c>
       <c r="O127" s="1" t="b">
-        <f>IF(N127&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P127" s="1" t="b">
@@ -14364,15 +14387,15 @@
         <v>126</v>
       </c>
       <c r="M128" s="2" t="str">
-        <f>_xlfn.CONCAT(I128,L128,J128)</f>
+        <f t="shared" si="9"/>
         <v>EVQLVESGGGLVQPGGSLRLSCAASGFNISSSSIHWVRQAPGKGLEWVASISSYSGYTYYADSVKGRFTISADTSKNTAYLQMNSLRAEDTAVYYCARGGHDLDGLYALDYWGQGTLVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCRASQSVSSAVAWYQQKPGKAPKLLIYSASSLYSGVPSRFSGSRSGTDFTLTISSLQPEDFATYYCQQYKYVPVTFGQGTKVEIK</v>
       </c>
       <c r="N128" s="4">
-        <f>LEN(M128)</f>
+        <f t="shared" si="10"/>
         <v>241</v>
       </c>
       <c r="O128" s="1" t="b">
-        <f>IF(N128&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P128" s="1" t="b">
@@ -14426,15 +14449,15 @@
         <v>126</v>
       </c>
       <c r="M129" s="2" t="str">
-        <f t="shared" ref="M129:M138" si="0">_xlfn.CONCAT(I129,L129,J129)</f>
+        <f t="shared" ref="M129:M138" si="12">_xlfn.CONCAT(I129,L129,J129)</f>
         <v>EVQLVESGGGLVKPGGSLKVSCAASGFTFSSYAMHWVRQAPGKGLEWVSYIWSGADSIGYADSVKGRFTISRDNAKNSLYLQMNSLRAGDTAVYYCARDDDAFDYWGQGTAVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCQASQDIRFYLNWYQQKPGKAPKLLISAASTLQSGVPSRFSGSGSGTDFTLTITSLQPEDFATYYCAGYVPSYTFGPGTKVDIK</v>
       </c>
       <c r="N129" s="4">
-        <f t="shared" ref="N129:N149" si="1">LEN(M129)</f>
+        <f t="shared" ref="N129:N138" si="13">LEN(M129)</f>
         <v>234</v>
       </c>
       <c r="O129" s="1" t="b">
-        <f t="shared" ref="O129:O138" si="2">IF(N129&lt;=250,TRUE,FALSE)</f>
+        <f t="shared" ref="O129:O138" si="14">IF(N129&lt;=250,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="P129" s="1" t="b">
@@ -14482,15 +14505,15 @@
         <v>126</v>
       </c>
       <c r="M130" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>EVQLVESGGGLVKPGGSLKVSCAASGFTFSSYSMHWVRQAPGKGLEWVSSIWSGADSTGYADSVKGRFTISRDNAKNSLYLQMNSLRAGDTAVYYCARDDDAFDYWGQGTAVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCQASQDIRFYLNWYQQKPGKAPKLLISAASTLQSGVPSRFSGSGSGTDFTLTITSLQPEDFATYYCAGYVPSYTFGPGTKVDIK</v>
       </c>
       <c r="N130" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>234</v>
       </c>
       <c r="O130" s="1" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="P130" s="1" t="b">
@@ -14538,15 +14561,15 @@
         <v>126</v>
       </c>
       <c r="M131" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>EVQLVESGGGLVKPGGSLKVSCAASGFTFSSYAMHWVRQAPGKGLEWVSRIWSGADSTGYADSVKGRFTISRDNAKNSLYLQMNSLRAGDTAVYYCARDDDAFDYWGQGTAVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCQASQDIRFYLNWYQQKPGKAPKLLISAASTLQSGVPSRFSGSGSGTDFTLTITSLQPEDFATYYCAGYVPSYTFGPGTKVDIK</v>
       </c>
       <c r="N131" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>234</v>
       </c>
       <c r="O131" s="1" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="P131" s="1" t="b">
@@ -14594,15 +14617,15 @@
         <v>126</v>
       </c>
       <c r="M132" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>EVQLVESGGGLVKPGGSLKVSCAASGFTFSSYAMHWVRQAPGKGLEWVSYIWSGADSIGYADSVKGRFTISRDNAKNSLYLQMNSLRAGDTAVYYCARYDDAFDYWGQGTAVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCQASQDIRFYLNWYQQKPGKAPKLLISAASTLQSGVPSRFSGSGSGTDFTLTITSLQPEDFATYYCAGYVPSYTFGPGTKVDIK</v>
       </c>
       <c r="N132" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>234</v>
       </c>
       <c r="O132" s="1" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="P132" s="1" t="b">
@@ -14650,15 +14673,15 @@
         <v>126</v>
       </c>
       <c r="M133" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>EVQLVESGGGLVKPGGSLKVSCAASGFTFSSYSMHWVRQAPGKGLEWVSRIWSGTDSIGYADSVKGRFTISRDNAKNSLYLQMNSLRAGDTAVYYCARDDDAFDYWGQGTAVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCQASQDIRFYLNWYQQKPGKAPKLLISAASTLQSGVPSRFSGSGSGTDFTLTITSLQPEDFATYYCAGYVPSYTFGPGTKVDIK</v>
       </c>
       <c r="N133" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>234</v>
       </c>
       <c r="O133" s="1" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="P133" s="1" t="b">
@@ -14706,15 +14729,15 @@
         <v>126</v>
       </c>
       <c r="M134" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>EVQLVESGGGLVKPGGSLKVSCAASGFTFSSYAMHWVRQAPGKGLEWVSYIWSGVDSIGYADSVKGRFTISRDNAKNSLYLQMNSLRAGDTAVYYCARDDDAFDYWGQGTAVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCQASQDIRFYLNWYQQKPGKAPKLLISAASTLQSGVPSRFSGSGSGTDFTLTITSLQPEDFATYYCAGYVPSYTFGPGTKVDIK</v>
       </c>
       <c r="N134" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>234</v>
       </c>
       <c r="O134" s="1" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="P134" s="1" t="b">
@@ -14762,15 +14785,15 @@
         <v>126</v>
       </c>
       <c r="M135" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>EVQLVESGGGLVKPGGSLKVSCAASGFTFSSFAMHWVRQAPGKGLEWVSYIWSGADSTGYADSVKGRFTISRDNAKNSLYLQMNSLRAGDTAVYYCARDDDAFDYWGQGTAVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCQASQDIRFYLNWYQQKPGKAPKLLISAASTLQSGVPSRFSGSGSGTDFTLTITSLQPEDFATYYCAGYVPSYTFGPGTKVDIK</v>
       </c>
       <c r="N135" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>234</v>
       </c>
       <c r="O135" s="1" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="P135" s="1" t="b">
@@ -14818,15 +14841,15 @@
         <v>126</v>
       </c>
       <c r="M136" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>EVQLVESGGGLVKPGGSLKVSCAASGFTFSSYAMHWVRQAPGKGLEWVSYIWSGADSIGYADSVKGRFTISRDNAKNSLYLQMNSLRAGDTAVYYCARYDDAFDYWGQGTAVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCQASQDIRFYLNWYQQKPGKAPKLLISAASTLQSGVPSRFSGSGSGTDFTLTITSLQPEDFATYYCAGYVPSYTFGPGTKVDIK</v>
       </c>
       <c r="N136" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>234</v>
       </c>
       <c r="O136" s="1" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="P136" s="1" t="b">
@@ -14874,15 +14897,15 @@
         <v>126</v>
       </c>
       <c r="M137" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>EVQLVESGGGLVKPGGSLKVSCAASGFTFSSYAMHWVRQAPGKGLEWVSYIWSGVDSIGYADSVKGRFTISRDNAKNSLYLQMNSLRAGDTAVYYCARDDDAFDYWGQGTAVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCQASQDIRFYLNWYQQKPGKAPKLLISAASTLQSGVPSRFSGSGSGTDFTLTITSLQPEDFATYYCAGYVPSYTFGPGTKVDIK</v>
       </c>
       <c r="N137" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>234</v>
       </c>
       <c r="O137" s="1" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="P137" s="1" t="b">
@@ -14930,15 +14953,15 @@
         <v>126</v>
       </c>
       <c r="M138" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>EVQLVESGGGLVKPGGSLKVSCAASGFTFSSYSMVWVRQAPGKGLEWVSRIWSGVDSTGYADSVKGRFTISRDNAKNSLYLQMNSLRAGDTAVYYCARDDDAFDYWGQGTAVTVSSGGGSGGGSGGGSDIQMTQSPSSLSASVGDRVTITCQASQDIRFYLNWYQQKPGKAPKLLISAASTLQSGVPSRFSGSGSGTDFTLTITSLQPEDFATYYCAGYVPSYTFGPGTKVDIK</v>
       </c>
       <c r="N138" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>234</v>
       </c>
       <c r="O138" s="1" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="P138" s="1" t="b">
@@ -14955,34 +14978,34 @@
   <autoFilter ref="A1:V118" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="K1:L1048576">
-    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="20" priority="21">
+    <cfRule type="containsBlanks" dxfId="22" priority="21">
       <formula>LEN(TRIM(K1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O138">
-    <cfRule type="containsBlanks" dxfId="19" priority="13">
+    <cfRule type="containsBlanks" dxfId="21" priority="13">
       <formula>LEN(TRIM(O2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O84:Q128 O129:O138">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+  <conditionalFormatting sqref="O84:Q138">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:S2 O3:Q83 R3:S22">
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="22" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14999,18 +15022,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:V22">
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P129:Q138">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15165,10 +15180,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F39314-0648-4D13-9FBE-8D5595154332}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15323,28 +15338,63 @@
         <v>5.3319999999999999E-3</v>
       </c>
     </row>
+    <row r="5" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="F5" s="2" t="str">
+        <f>_xlfn.CONCAT(C5,E5,D5)</f>
+        <v>EVQLVQSGAEVKKRGSSVKVSCKSSGGTFSNYAINWVRQAPGQGLEWMGGIIPILGIANYAQKFQGRVTITTDESTSTAYMELSSLRSEDTAVYYCARGWGREQLAPHPSQYYYYYYGMDVWGQGTTVTVSSGGGSGGGSGGGEIVMTQSPGTPSLSPGERATLSCRASQSIRSTYLAWYQQKPGQAPRLLIYGASSRATGIPDRFSGSGSGTDFTLTISRLEPEDFAVYYCQQYGRSPSFGQGTKVEIK</v>
+      </c>
+      <c r="G5" s="4">
+        <f>LEN(F5)</f>
+        <v>250</v>
+      </c>
+      <c r="H5" s="1" t="b">
+        <f>IF(G5&lt;=250,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.47112500000000002</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.66756800000000005</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E4">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+  <conditionalFormatting sqref="E1:E5">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
-    <cfRule type="containsBlanks" dxfId="10" priority="10">
+  <conditionalFormatting sqref="H2:H5">
+    <cfRule type="containsBlanks" dxfId="12" priority="16">
       <formula>LEN(TRIM(H2))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:J2">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -15356,14 +15406,50 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:J2">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="15" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:J3">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:J4">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -15374,14 +15460,14 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:J4">
+  <conditionalFormatting sqref="J5">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -15392,10 +15478,10 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>